<commit_message>
DQ3 - up to death in pyramid
</commit_message>
<xml_diff>
--- a/DW3/DQ3.xlsx
+++ b/DW3/DQ3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="233">
   <si>
     <t>Notes</t>
   </si>
@@ -724,9 +724,6 @@
     <t>To Cave</t>
   </si>
   <si>
-    <t>To Pyramid</t>
-  </si>
-  <si>
     <t>Up Stairs</t>
   </si>
   <si>
@@ -755,6 +752,12 @@
   </si>
   <si>
     <t>Enter Pyramid</t>
+  </si>
+  <si>
+    <t>Through Pyramid</t>
+  </si>
+  <si>
+    <t>Death</t>
   </si>
 </sst>
 </file>
@@ -2401,8 +2404,8 @@
   <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="6" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2431,7 +2434,7 @@
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65538)</f>
-        <v>0</v>
+        <v>7969</v>
       </c>
       <c r="I1" s="141" t="s">
         <v>202</v>
@@ -2453,19 +2456,19 @@
       <c r="G2" s="140"/>
       <c r="H2" s="144">
         <f>IF(H1&lt;3600,H1/60,QUOTIENT(H1, 3600))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="141" t="str">
         <f>IF(H1&lt;3600,"Seconds","Minutes")</f>
-        <v>Seconds</v>
-      </c>
-      <c r="J2" s="144" t="str">
+        <v>Minutes</v>
+      </c>
+      <c r="J2" s="144">
         <f>IF(H1&lt;3600,"",(MOD(H1,3600)/60))</f>
-        <v/>
+        <v>12.816666666666666</v>
       </c>
       <c r="K2" s="141" t="str">
         <f>IF(H1&lt;3600, "", "Seconds")</f>
-        <v/>
+        <v>Seconds</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="12.75" customHeight="1">
@@ -2719,7 +2722,7 @@
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
       <c r="A19" s="151" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="B19" s="109" t="s">
         <v>181</v>
@@ -2757,7 +2760,7 @@
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
       <c r="A21" s="150"/>
       <c r="B21" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C21" s="101">
         <v>9264</v>
@@ -2774,7 +2777,7 @@
     <row r="22" spans="1:7" ht="15" outlineLevel="1">
       <c r="A22" s="150"/>
       <c r="B22" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C22" s="101">
         <v>10006</v>
@@ -2791,7 +2794,7 @@
     <row r="23" spans="1:7" ht="15" outlineLevel="1">
       <c r="A23" s="150"/>
       <c r="B23" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C23" s="101">
         <v>11009</v>
@@ -2808,7 +2811,7 @@
     <row r="24" spans="1:7" ht="15" outlineLevel="1">
       <c r="A24" s="150"/>
       <c r="B24" s="148" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C24" s="101">
         <v>12082</v>
@@ -2825,7 +2828,7 @@
     <row r="25" spans="1:7" ht="15" outlineLevel="1">
       <c r="A25" s="150"/>
       <c r="B25" s="148" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C25" s="101">
         <v>13338</v>
@@ -2842,7 +2845,7 @@
     <row r="26" spans="1:7" ht="15" outlineLevel="1">
       <c r="A26" s="150"/>
       <c r="B26" s="148" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C26" s="101">
         <v>16018</v>
@@ -2859,7 +2862,7 @@
     <row r="27" spans="1:7" ht="15" outlineLevel="1">
       <c r="A27" s="150"/>
       <c r="B27" s="148" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C27" s="101">
         <v>17678</v>
@@ -2876,7 +2879,7 @@
     <row r="28" spans="1:7" ht="15" outlineLevel="1">
       <c r="A28" s="150"/>
       <c r="B28" s="148" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C28" s="101">
         <v>20692</v>
@@ -2893,7 +2896,7 @@
     <row r="29" spans="1:7" ht="15" outlineLevel="1">
       <c r="A29" s="150"/>
       <c r="B29" s="148" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C29" s="101">
         <v>23167</v>
@@ -2910,7 +2913,7 @@
     <row r="30" spans="1:7" ht="15" outlineLevel="1">
       <c r="A30" s="150"/>
       <c r="B30" s="148" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C30" s="101">
         <v>24630</v>
@@ -2927,7 +2930,7 @@
     <row r="31" spans="1:7" ht="15" outlineLevel="1">
       <c r="A31" s="150"/>
       <c r="B31" s="148" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C31" s="101"/>
       <c r="D31" s="101">
@@ -2942,7 +2945,7 @@
     <row r="32" spans="1:7" ht="15" outlineLevel="1">
       <c r="A32" s="150"/>
       <c r="B32" s="213" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C32" s="101">
         <v>27502</v>
@@ -2959,7 +2962,7 @@
     <row r="33" spans="1:7" ht="15" outlineLevel="1">
       <c r="A33" s="150"/>
       <c r="B33" s="213" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C33" s="101">
         <v>29241</v>
@@ -2976,7 +2979,7 @@
     <row r="34" spans="1:7" ht="15" outlineLevel="1">
       <c r="A34" s="150"/>
       <c r="B34" s="213" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C34" s="101">
         <v>30054</v>
@@ -2992,12 +2995,18 @@
     </row>
     <row r="35" spans="1:7" ht="15" outlineLevel="1">
       <c r="A35" s="150"/>
-      <c r="B35" s="100"/>
-      <c r="C35" s="101"/>
-      <c r="D35" s="101"/>
+      <c r="B35" s="213" t="s">
+        <v>232</v>
+      </c>
+      <c r="C35" s="101">
+        <v>34644</v>
+      </c>
+      <c r="D35" s="101">
+        <v>42613</v>
+      </c>
       <c r="E35" s="123">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7969</v>
       </c>
       <c r="F35" s="105"/>
     </row>
@@ -3006,11 +3015,15 @@
       <c r="B36" s="98" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
+      <c r="C36" s="99">
+        <v>34644</v>
+      </c>
+      <c r="D36" s="99">
+        <v>42613</v>
+      </c>
       <c r="E36" s="125">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7969</v>
       </c>
       <c r="F36" s="104"/>
     </row>
@@ -3023,20 +3036,20 @@
       </c>
       <c r="C37" s="103">
         <f>C36-C20</f>
-        <v>-8110</v>
+        <v>26534</v>
       </c>
       <c r="D37" s="103">
         <f>D36-D20</f>
-        <v>-10236</v>
+        <v>32377</v>
       </c>
       <c r="E37" s="126">
         <f>E36-E20</f>
-        <v>-2126</v>
+        <v>5843</v>
       </c>
       <c r="F37" s="108"/>
       <c r="G37" s="112">
         <f>E37</f>
-        <v>-2126</v>
+        <v>5843</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1"/>
@@ -25382,7 +25395,7 @@
       </c>
       <c r="C6" s="134">
         <f>FrameCounts!H2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
@@ -25394,7 +25407,7 @@
       </c>
       <c r="C7" s="135">
         <f>C6/60</f>
-        <v>0</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>

</xml_diff>

<commit_message>
DQ3 - at first enoucnter manipulation.  Must manipulation a 4 bomb crag fight.  Also added a text file of improvements for the next version.
</commit_message>
<xml_diff>
--- a/DW3/DQ3.xlsx
+++ b/DW3/DQ3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="235">
   <si>
     <t>Notes</t>
   </si>
@@ -762,6 +762,9 @@
   <si>
     <t>Beging registration</t>
   </si>
+  <si>
+    <t>Step on square to right of Kanave</t>
+  </si>
 </sst>
 </file>
 
@@ -771,10 +774,17 @@
     <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="47">
+  <fonts count="48">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1700,34 +1710,34 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="216">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1735,208 +1745,208 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="23" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="22" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="27" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="17" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="18" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="28" fillId="19" borderId="31" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="23" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="22" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="16" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="20" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="29" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="30" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="42" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1946,10 +1956,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1970,140 +1980,143 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="45" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="20" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="16" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="47" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -2418,7 +2431,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2434,16 +2447,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="156" t="s">
         <v>211</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="156" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="157" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="158"/>
       <c r="G1" s="140"/>
       <c r="H1" s="141">
         <f>SUM(G1:G65538)</f>
@@ -2521,10 +2534,10 @@
       <c r="B5" s="147" t="s">
         <v>183</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="154" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="153"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="147"/>
       <c r="F5" s="143"/>
       <c r="G5" s="140"/>
@@ -2540,10 +2553,10 @@
       <c r="B6" s="147" t="s">
         <v>186</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="154" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="147"/>
       <c r="F6" s="143"/>
       <c r="G6" s="140"/>
@@ -2561,7 +2574,7 @@
       <c r="F7" s="93"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A8" s="158" t="s">
+      <c r="A8" s="159" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="95" t="s">
@@ -2581,7 +2594,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A9" s="151"/>
+      <c r="A9" s="152"/>
       <c r="B9" s="98" t="s">
         <v>183</v>
       </c>
@@ -2595,7 +2608,7 @@
       <c r="F9" s="104"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A10" s="151"/>
+      <c r="A10" s="152"/>
       <c r="B10" s="148" t="s">
         <v>215</v>
       </c>
@@ -2612,7 +2625,7 @@
       <c r="F10" s="105"/>
     </row>
     <row r="11" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A11" s="151"/>
+      <c r="A11" s="152"/>
       <c r="B11" s="148" t="s">
         <v>216</v>
       </c>
@@ -2629,7 +2642,7 @@
       <c r="F11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A12" s="151"/>
+      <c r="A12" s="152"/>
       <c r="B12" s="148" t="s">
         <v>217</v>
       </c>
@@ -2646,7 +2659,7 @@
       <c r="F12" s="105"/>
     </row>
     <row r="13" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A13" s="151"/>
+      <c r="A13" s="152"/>
       <c r="B13" s="148" t="s">
         <v>218</v>
       </c>
@@ -2663,7 +2676,7 @@
       <c r="F13" s="105"/>
     </row>
     <row r="14" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A14" s="151"/>
+      <c r="A14" s="152"/>
       <c r="B14" s="148" t="s">
         <v>219</v>
       </c>
@@ -2680,7 +2693,7 @@
       <c r="F14" s="105"/>
     </row>
     <row r="15" spans="1:11" ht="15" outlineLevel="1">
-      <c r="A15" s="151"/>
+      <c r="A15" s="152"/>
       <c r="B15" s="100"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
@@ -2691,7 +2704,7 @@
       <c r="F15" s="105"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A16" s="151"/>
+      <c r="A16" s="152"/>
       <c r="B16" s="98" t="s">
         <v>186</v>
       </c>
@@ -2734,7 +2747,7 @@
     </row>
     <row r="18" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="19" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A19" s="152" t="s">
+      <c r="A19" s="153" t="s">
         <v>231</v>
       </c>
       <c r="B19" s="109" t="s">
@@ -2754,7 +2767,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A20" s="151"/>
+      <c r="A20" s="152"/>
       <c r="B20" s="98" t="s">
         <v>183</v>
       </c>
@@ -2771,7 +2784,7 @@
       <c r="F20" s="104"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A21" s="151"/>
+      <c r="A21" s="152"/>
       <c r="B21" s="148" t="s">
         <v>221</v>
       </c>
@@ -2788,7 +2801,7 @@
       <c r="F21" s="105"/>
     </row>
     <row r="22" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A22" s="151"/>
+      <c r="A22" s="152"/>
       <c r="B22" s="148" t="s">
         <v>221</v>
       </c>
@@ -2805,7 +2818,7 @@
       <c r="F22" s="105"/>
     </row>
     <row r="23" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A23" s="151"/>
+      <c r="A23" s="152"/>
       <c r="B23" s="148" t="s">
         <v>221</v>
       </c>
@@ -2822,7 +2835,7 @@
       <c r="F23" s="105"/>
     </row>
     <row r="24" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A24" s="151"/>
+      <c r="A24" s="152"/>
       <c r="B24" s="148" t="s">
         <v>221</v>
       </c>
@@ -2839,7 +2852,7 @@
       <c r="F24" s="105"/>
     </row>
     <row r="25" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A25" s="151"/>
+      <c r="A25" s="152"/>
       <c r="B25" s="148" t="s">
         <v>222</v>
       </c>
@@ -2856,7 +2869,7 @@
       <c r="F25" s="105"/>
     </row>
     <row r="26" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A26" s="151"/>
+      <c r="A26" s="152"/>
       <c r="B26" s="148" t="s">
         <v>223</v>
       </c>
@@ -2873,7 +2886,7 @@
       <c r="F26" s="105"/>
     </row>
     <row r="27" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A27" s="151"/>
+      <c r="A27" s="152"/>
       <c r="B27" s="148" t="s">
         <v>224</v>
       </c>
@@ -2890,7 +2903,7 @@
       <c r="F27" s="105"/>
     </row>
     <row r="28" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A28" s="151"/>
+      <c r="A28" s="152"/>
       <c r="B28" s="148" t="s">
         <v>224</v>
       </c>
@@ -2907,7 +2920,7 @@
       <c r="F28" s="105"/>
     </row>
     <row r="29" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A29" s="151"/>
+      <c r="A29" s="152"/>
       <c r="B29" s="148" t="s">
         <v>225</v>
       </c>
@@ -2924,7 +2937,7 @@
       <c r="F29" s="105"/>
     </row>
     <row r="30" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A30" s="151"/>
+      <c r="A30" s="152"/>
       <c r="B30" s="148" t="s">
         <v>226</v>
       </c>
@@ -2941,7 +2954,7 @@
       <c r="F30" s="105"/>
     </row>
     <row r="31" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A31" s="151"/>
+      <c r="A31" s="152"/>
       <c r="B31" s="148" t="s">
         <v>227</v>
       </c>
@@ -2956,7 +2969,7 @@
       <c r="F31" s="105"/>
     </row>
     <row r="32" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A32" s="151"/>
+      <c r="A32" s="152"/>
       <c r="B32" s="149" t="s">
         <v>228</v>
       </c>
@@ -2973,7 +2986,7 @@
       <c r="F32" s="105"/>
     </row>
     <row r="33" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A33" s="151"/>
+      <c r="A33" s="152"/>
       <c r="B33" s="149" t="s">
         <v>229</v>
       </c>
@@ -2990,7 +3003,7 @@
       <c r="F33" s="105"/>
     </row>
     <row r="34" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A34" s="151"/>
+      <c r="A34" s="152"/>
       <c r="B34" s="149" t="s">
         <v>230</v>
       </c>
@@ -3007,7 +3020,7 @@
       <c r="F34" s="105"/>
     </row>
     <row r="35" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A35" s="151"/>
+      <c r="A35" s="152"/>
       <c r="B35" s="149" t="s">
         <v>232</v>
       </c>
@@ -3024,7 +3037,7 @@
       <c r="F35" s="105"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A36" s="151"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="98" t="s">
         <v>186</v>
       </c>
@@ -3067,7 +3080,7 @@
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="39" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A39" s="150" t="s">
+      <c r="A39" s="151" t="s">
         <v>169</v>
       </c>
       <c r="B39" s="113" t="s">
@@ -3087,7 +3100,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A40" s="151"/>
+      <c r="A40" s="152"/>
       <c r="B40" s="98" t="s">
         <v>183</v>
       </c>
@@ -3104,8 +3117,8 @@
       <c r="F40" s="104"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A41" s="151"/>
-      <c r="B41" s="214" t="s">
+      <c r="A41" s="152"/>
+      <c r="B41" s="150" t="s">
         <v>233</v>
       </c>
       <c r="C41" s="101">
@@ -3121,18 +3134,24 @@
       <c r="F41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A42" s="151"/>
-      <c r="B42" s="100"/>
-      <c r="C42" s="101"/>
-      <c r="D42" s="101"/>
+      <c r="A42" s="152"/>
+      <c r="B42" s="215" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="101">
+        <v>41709</v>
+      </c>
+      <c r="D42" s="101">
+        <v>67224</v>
+      </c>
       <c r="E42" s="123">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>25515</v>
       </c>
       <c r="F42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A43" s="151"/>
+      <c r="A43" s="152"/>
       <c r="B43" s="100"/>
       <c r="C43" s="101"/>
       <c r="D43" s="101"/>
@@ -3143,7 +3162,7 @@
       <c r="F43" s="105"/>
     </row>
     <row r="44" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A44" s="151"/>
+      <c r="A44" s="152"/>
       <c r="B44" s="100"/>
       <c r="C44" s="101"/>
       <c r="D44" s="101"/>
@@ -3154,7 +3173,7 @@
       <c r="F44" s="105"/>
     </row>
     <row r="45" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A45" s="151"/>
+      <c r="A45" s="152"/>
       <c r="B45" s="100"/>
       <c r="C45" s="101"/>
       <c r="D45" s="101"/>
@@ -3165,7 +3184,7 @@
       <c r="F45" s="105"/>
     </row>
     <row r="46" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A46" s="151"/>
+      <c r="A46" s="152"/>
       <c r="B46" s="100"/>
       <c r="C46" s="101"/>
       <c r="D46" s="101"/>
@@ -3176,7 +3195,7 @@
       <c r="F46" s="105"/>
     </row>
     <row r="47" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A47" s="151"/>
+      <c r="A47" s="152"/>
       <c r="B47" s="100"/>
       <c r="C47" s="101"/>
       <c r="D47" s="101"/>
@@ -3187,7 +3206,7 @@
       <c r="F47" s="105"/>
     </row>
     <row r="48" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A48" s="151"/>
+      <c r="A48" s="152"/>
       <c r="B48" s="100"/>
       <c r="C48" s="101"/>
       <c r="D48" s="101"/>
@@ -3198,7 +3217,7 @@
       <c r="F48" s="105"/>
     </row>
     <row r="49" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A49" s="151"/>
+      <c r="A49" s="152"/>
       <c r="B49" s="100"/>
       <c r="C49" s="101"/>
       <c r="D49" s="101"/>
@@ -3209,7 +3228,7 @@
       <c r="F49" s="105"/>
     </row>
     <row r="50" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A50" s="151"/>
+      <c r="A50" s="152"/>
       <c r="B50" s="100"/>
       <c r="C50" s="101"/>
       <c r="D50" s="101"/>
@@ -3220,7 +3239,7 @@
       <c r="F50" s="105"/>
     </row>
     <row r="51" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A51" s="151"/>
+      <c r="A51" s="152"/>
       <c r="B51" s="100"/>
       <c r="C51" s="101"/>
       <c r="D51" s="101"/>
@@ -3231,7 +3250,7 @@
       <c r="F51" s="105"/>
     </row>
     <row r="52" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A52" s="151"/>
+      <c r="A52" s="152"/>
       <c r="B52" s="100"/>
       <c r="C52" s="101"/>
       <c r="D52" s="101"/>
@@ -3242,7 +3261,7 @@
       <c r="F52" s="105"/>
     </row>
     <row r="53" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A53" s="151"/>
+      <c r="A53" s="152"/>
       <c r="B53" s="98" t="s">
         <v>186</v>
       </c>
@@ -3281,7 +3300,7 @@
     </row>
     <row r="55" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="56" spans="1:7" ht="15" customHeight="1" outlineLevel="1">
-      <c r="A56" s="152" t="s">
+      <c r="A56" s="153" t="s">
         <v>170</v>
       </c>
       <c r="B56" s="109" t="s">
@@ -3301,7 +3320,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A57" s="151"/>
+      <c r="A57" s="152"/>
       <c r="B57" s="98" t="s">
         <v>183</v>
       </c>
@@ -3314,7 +3333,7 @@
       <c r="F57" s="104"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" outlineLevel="1" thickTop="1">
-      <c r="A58" s="151"/>
+      <c r="A58" s="152"/>
       <c r="B58" s="100"/>
       <c r="C58" s="101"/>
       <c r="D58" s="101"/>
@@ -3325,7 +3344,7 @@
       <c r="F58" s="105"/>
     </row>
     <row r="59" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A59" s="151"/>
+      <c r="A59" s="152"/>
       <c r="B59" s="100"/>
       <c r="C59" s="101"/>
       <c r="D59" s="101"/>
@@ -3336,7 +3355,7 @@
       <c r="F59" s="105"/>
     </row>
     <row r="60" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A60" s="151"/>
+      <c r="A60" s="152"/>
       <c r="B60" s="100"/>
       <c r="C60" s="101"/>
       <c r="D60" s="101"/>
@@ -3347,7 +3366,7 @@
       <c r="F60" s="105"/>
     </row>
     <row r="61" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A61" s="151"/>
+      <c r="A61" s="152"/>
       <c r="B61" s="100"/>
       <c r="C61" s="101"/>
       <c r="D61" s="101"/>
@@ -3358,7 +3377,7 @@
       <c r="F61" s="105"/>
     </row>
     <row r="62" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A62" s="151"/>
+      <c r="A62" s="152"/>
       <c r="B62" s="100"/>
       <c r="C62" s="101"/>
       <c r="D62" s="101"/>
@@ -3369,7 +3388,7 @@
       <c r="F62" s="105"/>
     </row>
     <row r="63" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A63" s="151"/>
+      <c r="A63" s="152"/>
       <c r="B63" s="100"/>
       <c r="C63" s="101"/>
       <c r="D63" s="101"/>
@@ -3380,7 +3399,7 @@
       <c r="F63" s="105"/>
     </row>
     <row r="64" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A64" s="151"/>
+      <c r="A64" s="152"/>
       <c r="B64" s="100"/>
       <c r="C64" s="101"/>
       <c r="D64" s="101"/>
@@ -3391,7 +3410,7 @@
       <c r="F64" s="105"/>
     </row>
     <row r="65" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A65" s="151"/>
+      <c r="A65" s="152"/>
       <c r="B65" s="100"/>
       <c r="C65" s="101"/>
       <c r="D65" s="101"/>
@@ -3402,7 +3421,7 @@
       <c r="F65" s="105"/>
     </row>
     <row r="66" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A66" s="151"/>
+      <c r="A66" s="152"/>
       <c r="B66" s="100"/>
       <c r="C66" s="101"/>
       <c r="D66" s="101"/>
@@ -3413,7 +3432,7 @@
       <c r="F66" s="105"/>
     </row>
     <row r="67" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A67" s="151"/>
+      <c r="A67" s="152"/>
       <c r="B67" s="100"/>
       <c r="C67" s="101"/>
       <c r="D67" s="101"/>
@@ -3424,7 +3443,7 @@
       <c r="F67" s="105"/>
     </row>
     <row r="68" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A68" s="151"/>
+      <c r="A68" s="152"/>
       <c r="B68" s="100"/>
       <c r="C68" s="101"/>
       <c r="D68" s="101"/>
@@ -3435,7 +3454,7 @@
       <c r="F68" s="105"/>
     </row>
     <row r="69" spans="1:7" ht="15" outlineLevel="1">
-      <c r="A69" s="151"/>
+      <c r="A69" s="152"/>
       <c r="B69" s="100"/>
       <c r="C69" s="101"/>
       <c r="D69" s="101"/>
@@ -3446,7 +3465,7 @@
       <c r="F69" s="105"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" outlineLevel="1" thickBot="1">
-      <c r="A70" s="151"/>
+      <c r="A70" s="152"/>
       <c r="B70" s="98" t="s">
         <v>186</v>
       </c>
@@ -3485,7 +3504,7 @@
     </row>
     <row r="72" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="73" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A73" s="150" t="s">
+      <c r="A73" s="151" t="s">
         <v>171</v>
       </c>
       <c r="B73" s="113" t="s">
@@ -3505,7 +3524,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A74" s="151"/>
+      <c r="A74" s="152"/>
       <c r="B74" s="98" t="s">
         <v>183</v>
       </c>
@@ -3518,7 +3537,7 @@
       <c r="F74" s="104"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A75" s="151"/>
+      <c r="A75" s="152"/>
       <c r="B75" s="100"/>
       <c r="C75" s="101"/>
       <c r="D75" s="101"/>
@@ -3529,7 +3548,7 @@
       <c r="F75" s="105"/>
     </row>
     <row r="76" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A76" s="151"/>
+      <c r="A76" s="152"/>
       <c r="B76" s="100"/>
       <c r="C76" s="101"/>
       <c r="D76" s="101"/>
@@ -3540,7 +3559,7 @@
       <c r="F76" s="105"/>
     </row>
     <row r="77" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A77" s="151"/>
+      <c r="A77" s="152"/>
       <c r="B77" s="100"/>
       <c r="C77" s="101"/>
       <c r="D77" s="101"/>
@@ -3551,7 +3570,7 @@
       <c r="F77" s="105"/>
     </row>
     <row r="78" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A78" s="151"/>
+      <c r="A78" s="152"/>
       <c r="B78" s="100"/>
       <c r="C78" s="101"/>
       <c r="D78" s="101"/>
@@ -3562,7 +3581,7 @@
       <c r="F78" s="105"/>
     </row>
     <row r="79" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A79" s="151"/>
+      <c r="A79" s="152"/>
       <c r="B79" s="100"/>
       <c r="C79" s="101"/>
       <c r="D79" s="101"/>
@@ -3573,7 +3592,7 @@
       <c r="F79" s="105"/>
     </row>
     <row r="80" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A80" s="151"/>
+      <c r="A80" s="152"/>
       <c r="B80" s="100"/>
       <c r="C80" s="101"/>
       <c r="D80" s="101"/>
@@ -3584,7 +3603,7 @@
       <c r="F80" s="105"/>
     </row>
     <row r="81" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A81" s="151"/>
+      <c r="A81" s="152"/>
       <c r="B81" s="100"/>
       <c r="C81" s="101"/>
       <c r="D81" s="101"/>
@@ -3595,7 +3614,7 @@
       <c r="F81" s="105"/>
     </row>
     <row r="82" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A82" s="151"/>
+      <c r="A82" s="152"/>
       <c r="B82" s="100"/>
       <c r="C82" s="101"/>
       <c r="D82" s="101"/>
@@ -3606,7 +3625,7 @@
       <c r="F82" s="105"/>
     </row>
     <row r="83" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A83" s="151"/>
+      <c r="A83" s="152"/>
       <c r="B83" s="100"/>
       <c r="C83" s="101"/>
       <c r="D83" s="101"/>
@@ -3617,7 +3636,7 @@
       <c r="F83" s="105"/>
     </row>
     <row r="84" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A84" s="151"/>
+      <c r="A84" s="152"/>
       <c r="B84" s="100"/>
       <c r="C84" s="101"/>
       <c r="D84" s="101"/>
@@ -3628,7 +3647,7 @@
       <c r="F84" s="105"/>
     </row>
     <row r="85" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A85" s="151"/>
+      <c r="A85" s="152"/>
       <c r="B85" s="100"/>
       <c r="C85" s="101"/>
       <c r="D85" s="101"/>
@@ -3639,7 +3658,7 @@
       <c r="F85" s="105"/>
     </row>
     <row r="86" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A86" s="151"/>
+      <c r="A86" s="152"/>
       <c r="B86" s="100"/>
       <c r="C86" s="101"/>
       <c r="D86" s="101"/>
@@ -3650,7 +3669,7 @@
       <c r="F86" s="105"/>
     </row>
     <row r="87" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A87" s="151"/>
+      <c r="A87" s="152"/>
       <c r="B87" s="98" t="s">
         <v>186</v>
       </c>
@@ -3689,7 +3708,7 @@
     </row>
     <row r="89" spans="1:7" ht="13.5" thickBot="1"/>
     <row r="90" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A90" s="152" t="s">
+      <c r="A90" s="153" t="s">
         <v>172</v>
       </c>
       <c r="B90" s="109" t="s">
@@ -3709,7 +3728,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A91" s="151"/>
+      <c r="A91" s="152"/>
       <c r="B91" s="98" t="s">
         <v>183</v>
       </c>
@@ -3722,7 +3741,7 @@
       <c r="F91" s="104"/>
     </row>
     <row r="92" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A92" s="151"/>
+      <c r="A92" s="152"/>
       <c r="B92" s="100"/>
       <c r="C92" s="101"/>
       <c r="D92" s="101"/>
@@ -3733,7 +3752,7 @@
       <c r="F92" s="105"/>
     </row>
     <row r="93" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A93" s="151"/>
+      <c r="A93" s="152"/>
       <c r="B93" s="100"/>
       <c r="C93" s="101"/>
       <c r="D93" s="101"/>
@@ -3744,7 +3763,7 @@
       <c r="F93" s="105"/>
     </row>
     <row r="94" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A94" s="151"/>
+      <c r="A94" s="152"/>
       <c r="B94" s="100"/>
       <c r="C94" s="101"/>
       <c r="D94" s="101"/>
@@ -3755,7 +3774,7 @@
       <c r="F94" s="105"/>
     </row>
     <row r="95" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A95" s="151"/>
+      <c r="A95" s="152"/>
       <c r="B95" s="100"/>
       <c r="C95" s="101"/>
       <c r="D95" s="101"/>
@@ -3766,7 +3785,7 @@
       <c r="F95" s="105"/>
     </row>
     <row r="96" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A96" s="151"/>
+      <c r="A96" s="152"/>
       <c r="B96" s="100"/>
       <c r="C96" s="101"/>
       <c r="D96" s="101"/>
@@ -3777,7 +3796,7 @@
       <c r="F96" s="105"/>
     </row>
     <row r="97" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A97" s="151"/>
+      <c r="A97" s="152"/>
       <c r="B97" s="100"/>
       <c r="C97" s="101"/>
       <c r="D97" s="101"/>
@@ -3788,7 +3807,7 @@
       <c r="F97" s="105"/>
     </row>
     <row r="98" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A98" s="151"/>
+      <c r="A98" s="152"/>
       <c r="B98" s="100"/>
       <c r="C98" s="101"/>
       <c r="D98" s="101"/>
@@ -3799,7 +3818,7 @@
       <c r="F98" s="105"/>
     </row>
     <row r="99" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A99" s="151"/>
+      <c r="A99" s="152"/>
       <c r="B99" s="100"/>
       <c r="C99" s="101"/>
       <c r="D99" s="101"/>
@@ -3810,7 +3829,7 @@
       <c r="F99" s="105"/>
     </row>
     <row r="100" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A100" s="151"/>
+      <c r="A100" s="152"/>
       <c r="B100" s="100"/>
       <c r="C100" s="101"/>
       <c r="D100" s="101"/>
@@ -3821,7 +3840,7 @@
       <c r="F100" s="105"/>
     </row>
     <row r="101" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A101" s="151"/>
+      <c r="A101" s="152"/>
       <c r="B101" s="100"/>
       <c r="C101" s="101"/>
       <c r="D101" s="101"/>
@@ -3832,7 +3851,7 @@
       <c r="F101" s="105"/>
     </row>
     <row r="102" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A102" s="151"/>
+      <c r="A102" s="152"/>
       <c r="B102" s="100"/>
       <c r="C102" s="101"/>
       <c r="D102" s="101"/>
@@ -3843,7 +3862,7 @@
       <c r="F102" s="105"/>
     </row>
     <row r="103" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A103" s="151"/>
+      <c r="A103" s="152"/>
       <c r="B103" s="100"/>
       <c r="C103" s="101"/>
       <c r="D103" s="101"/>
@@ -3854,7 +3873,7 @@
       <c r="F103" s="105"/>
     </row>
     <row r="104" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A104" s="151"/>
+      <c r="A104" s="152"/>
       <c r="B104" s="98" t="s">
         <v>186</v>
       </c>
@@ -3892,7 +3911,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A107" s="150" t="s">
+      <c r="A107" s="151" t="s">
         <v>173</v>
       </c>
       <c r="B107" s="113" t="s">
@@ -3912,7 +3931,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A108" s="151"/>
+      <c r="A108" s="152"/>
       <c r="B108" s="98" t="s">
         <v>183</v>
       </c>
@@ -3925,7 +3944,7 @@
       <c r="F108" s="104"/>
     </row>
     <row r="109" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A109" s="151"/>
+      <c r="A109" s="152"/>
       <c r="B109" s="100"/>
       <c r="C109" s="101"/>
       <c r="D109" s="101"/>
@@ -3936,7 +3955,7 @@
       <c r="F109" s="105"/>
     </row>
     <row r="110" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A110" s="151"/>
+      <c r="A110" s="152"/>
       <c r="B110" s="100"/>
       <c r="C110" s="101"/>
       <c r="D110" s="101"/>
@@ -3947,7 +3966,7 @@
       <c r="F110" s="105"/>
     </row>
     <row r="111" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A111" s="151"/>
+      <c r="A111" s="152"/>
       <c r="B111" s="100"/>
       <c r="C111" s="101"/>
       <c r="D111" s="101"/>
@@ -3958,7 +3977,7 @@
       <c r="F111" s="105"/>
     </row>
     <row r="112" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A112" s="151"/>
+      <c r="A112" s="152"/>
       <c r="B112" s="100"/>
       <c r="C112" s="101"/>
       <c r="D112" s="101"/>
@@ -3969,7 +3988,7 @@
       <c r="F112" s="105"/>
     </row>
     <row r="113" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A113" s="151"/>
+      <c r="A113" s="152"/>
       <c r="B113" s="100"/>
       <c r="C113" s="101"/>
       <c r="D113" s="101"/>
@@ -3980,7 +3999,7 @@
       <c r="F113" s="105"/>
     </row>
     <row r="114" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A114" s="151"/>
+      <c r="A114" s="152"/>
       <c r="B114" s="100"/>
       <c r="C114" s="101"/>
       <c r="D114" s="101"/>
@@ -3991,7 +4010,7 @@
       <c r="F114" s="105"/>
     </row>
     <row r="115" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A115" s="151"/>
+      <c r="A115" s="152"/>
       <c r="B115" s="100"/>
       <c r="C115" s="101"/>
       <c r="D115" s="101"/>
@@ -4002,7 +4021,7 @@
       <c r="F115" s="105"/>
     </row>
     <row r="116" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A116" s="151"/>
+      <c r="A116" s="152"/>
       <c r="B116" s="100"/>
       <c r="C116" s="101"/>
       <c r="D116" s="101"/>
@@ -4013,7 +4032,7 @@
       <c r="F116" s="105"/>
     </row>
     <row r="117" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A117" s="151"/>
+      <c r="A117" s="152"/>
       <c r="B117" s="100"/>
       <c r="C117" s="101"/>
       <c r="D117" s="101"/>
@@ -4024,7 +4043,7 @@
       <c r="F117" s="105"/>
     </row>
     <row r="118" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A118" s="151"/>
+      <c r="A118" s="152"/>
       <c r="B118" s="100"/>
       <c r="C118" s="101"/>
       <c r="D118" s="101"/>
@@ -4035,7 +4054,7 @@
       <c r="F118" s="105"/>
     </row>
     <row r="119" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A119" s="151"/>
+      <c r="A119" s="152"/>
       <c r="B119" s="100"/>
       <c r="C119" s="101"/>
       <c r="D119" s="101"/>
@@ -4046,7 +4065,7 @@
       <c r="F119" s="105"/>
     </row>
     <row r="120" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A120" s="151"/>
+      <c r="A120" s="152"/>
       <c r="B120" s="100"/>
       <c r="C120" s="101"/>
       <c r="D120" s="101"/>
@@ -4057,7 +4076,7 @@
       <c r="F120" s="105"/>
     </row>
     <row r="121" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A121" s="151"/>
+      <c r="A121" s="152"/>
       <c r="B121" s="98" t="s">
         <v>186</v>
       </c>
@@ -4095,7 +4114,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A124" s="152" t="s">
+      <c r="A124" s="153" t="s">
         <v>174</v>
       </c>
       <c r="B124" s="109" t="s">
@@ -4115,7 +4134,7 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A125" s="151"/>
+      <c r="A125" s="152"/>
       <c r="B125" s="98" t="s">
         <v>183</v>
       </c>
@@ -4128,7 +4147,7 @@
       <c r="F125" s="104"/>
     </row>
     <row r="126" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickTop="1">
-      <c r="A126" s="151"/>
+      <c r="A126" s="152"/>
       <c r="B126" s="100"/>
       <c r="C126" s="101"/>
       <c r="D126" s="101"/>
@@ -4139,7 +4158,7 @@
       <c r="F126" s="105"/>
     </row>
     <row r="127" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A127" s="151"/>
+      <c r="A127" s="152"/>
       <c r="B127" s="100"/>
       <c r="C127" s="101"/>
       <c r="D127" s="101"/>
@@ -4150,7 +4169,7 @@
       <c r="F127" s="105"/>
     </row>
     <row r="128" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A128" s="151"/>
+      <c r="A128" s="152"/>
       <c r="B128" s="100"/>
       <c r="C128" s="101"/>
       <c r="D128" s="101"/>
@@ -4161,7 +4180,7 @@
       <c r="F128" s="105"/>
     </row>
     <row r="129" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A129" s="151"/>
+      <c r="A129" s="152"/>
       <c r="B129" s="100"/>
       <c r="C129" s="101"/>
       <c r="D129" s="101"/>
@@ -4172,7 +4191,7 @@
       <c r="F129" s="105"/>
     </row>
     <row r="130" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A130" s="151"/>
+      <c r="A130" s="152"/>
       <c r="B130" s="100"/>
       <c r="C130" s="101"/>
       <c r="D130" s="101"/>
@@ -4183,7 +4202,7 @@
       <c r="F130" s="105"/>
     </row>
     <row r="131" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A131" s="151"/>
+      <c r="A131" s="152"/>
       <c r="B131" s="100"/>
       <c r="C131" s="101"/>
       <c r="D131" s="101"/>
@@ -4194,7 +4213,7 @@
       <c r="F131" s="105"/>
     </row>
     <row r="132" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A132" s="151"/>
+      <c r="A132" s="152"/>
       <c r="B132" s="100"/>
       <c r="C132" s="101"/>
       <c r="D132" s="101"/>
@@ -4205,7 +4224,7 @@
       <c r="F132" s="105"/>
     </row>
     <row r="133" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A133" s="151"/>
+      <c r="A133" s="152"/>
       <c r="B133" s="100"/>
       <c r="C133" s="101"/>
       <c r="D133" s="101"/>
@@ -4216,7 +4235,7 @@
       <c r="F133" s="105"/>
     </row>
     <row r="134" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A134" s="151"/>
+      <c r="A134" s="152"/>
       <c r="B134" s="100"/>
       <c r="C134" s="101"/>
       <c r="D134" s="101"/>
@@ -4227,7 +4246,7 @@
       <c r="F134" s="105"/>
     </row>
     <row r="135" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A135" s="151"/>
+      <c r="A135" s="152"/>
       <c r="B135" s="100"/>
       <c r="C135" s="101"/>
       <c r="D135" s="101"/>
@@ -4238,7 +4257,7 @@
       <c r="F135" s="105"/>
     </row>
     <row r="136" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A136" s="151"/>
+      <c r="A136" s="152"/>
       <c r="B136" s="100"/>
       <c r="C136" s="101"/>
       <c r="D136" s="101"/>
@@ -4249,7 +4268,7 @@
       <c r="F136" s="105"/>
     </row>
     <row r="137" spans="1:7" ht="15" hidden="1" outlineLevel="1">
-      <c r="A137" s="151"/>
+      <c r="A137" s="152"/>
       <c r="B137" s="100"/>
       <c r="C137" s="101"/>
       <c r="D137" s="101"/>
@@ -4260,7 +4279,7 @@
       <c r="F137" s="105"/>
     </row>
     <row r="138" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1">
-      <c r="A138" s="151"/>
+      <c r="A138" s="152"/>
       <c r="B138" s="98" t="s">
         <v>186</v>
       </c>
@@ -4298,7 +4317,7 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A141" s="150" t="s">
+      <c r="A141" s="151" t="s">
         <v>175</v>
       </c>
       <c r="B141" s="113" t="s">
@@ -4318,7 +4337,7 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A142" s="151"/>
+      <c r="A142" s="152"/>
       <c r="B142" s="98" t="s">
         <v>183</v>
       </c>
@@ -4331,7 +4350,7 @@
       <c r="F142" s="104"/>
     </row>
     <row r="143" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickTop="1">
-      <c r="A143" s="151"/>
+      <c r="A143" s="152"/>
       <c r="B143" s="100"/>
       <c r="C143" s="101"/>
       <c r="D143" s="101"/>
@@ -4342,7 +4361,7 @@
       <c r="F143" s="105"/>
     </row>
     <row r="144" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A144" s="151"/>
+      <c r="A144" s="152"/>
       <c r="B144" s="100"/>
       <c r="C144" s="101"/>
       <c r="D144" s="101"/>
@@ -4353,7 +4372,7 @@
       <c r="F144" s="105"/>
     </row>
     <row r="145" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A145" s="151"/>
+      <c r="A145" s="152"/>
       <c r="B145" s="100"/>
       <c r="C145" s="101"/>
       <c r="D145" s="101"/>
@@ -4364,7 +4383,7 @@
       <c r="F145" s="105"/>
     </row>
     <row r="146" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A146" s="151"/>
+      <c r="A146" s="152"/>
       <c r="B146" s="100"/>
       <c r="C146" s="101"/>
       <c r="D146" s="101"/>
@@ -4375,7 +4394,7 @@
       <c r="F146" s="105"/>
     </row>
     <row r="147" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A147" s="151"/>
+      <c r="A147" s="152"/>
       <c r="B147" s="100"/>
       <c r="C147" s="101"/>
       <c r="D147" s="101"/>
@@ -4386,7 +4405,7 @@
       <c r="F147" s="105"/>
     </row>
     <row r="148" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A148" s="151"/>
+      <c r="A148" s="152"/>
       <c r="B148" s="100"/>
       <c r="C148" s="101"/>
       <c r="D148" s="101"/>
@@ -4397,7 +4416,7 @@
       <c r="F148" s="105"/>
     </row>
     <row r="149" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A149" s="151"/>
+      <c r="A149" s="152"/>
       <c r="B149" s="100"/>
       <c r="C149" s="101"/>
       <c r="D149" s="101"/>
@@ -4408,7 +4427,7 @@
       <c r="F149" s="105"/>
     </row>
     <row r="150" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A150" s="151"/>
+      <c r="A150" s="152"/>
       <c r="B150" s="100"/>
       <c r="C150" s="101"/>
       <c r="D150" s="101"/>
@@ -4419,7 +4438,7 @@
       <c r="F150" s="105"/>
     </row>
     <row r="151" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A151" s="151"/>
+      <c r="A151" s="152"/>
       <c r="B151" s="100"/>
       <c r="C151" s="101"/>
       <c r="D151" s="101"/>
@@ -4430,7 +4449,7 @@
       <c r="F151" s="105"/>
     </row>
     <row r="152" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A152" s="151"/>
+      <c r="A152" s="152"/>
       <c r="B152" s="100"/>
       <c r="C152" s="101"/>
       <c r="D152" s="101"/>
@@ -4441,7 +4460,7 @@
       <c r="F152" s="105"/>
     </row>
     <row r="153" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A153" s="151"/>
+      <c r="A153" s="152"/>
       <c r="B153" s="100"/>
       <c r="C153" s="101"/>
       <c r="D153" s="101"/>
@@ -4452,7 +4471,7 @@
       <c r="F153" s="105"/>
     </row>
     <row r="154" spans="1:7" ht="15" hidden="1" outlineLevel="2">
-      <c r="A154" s="151"/>
+      <c r="A154" s="152"/>
       <c r="B154" s="100"/>
       <c r="C154" s="101"/>
       <c r="D154" s="101"/>
@@ -4463,7 +4482,7 @@
       <c r="F154" s="105"/>
     </row>
     <row r="155" spans="1:7" ht="15.75" hidden="1" outlineLevel="2" thickBot="1">
-      <c r="A155" s="151"/>
+      <c r="A155" s="152"/>
       <c r="B155" s="98" t="s">
         <v>186</v>
       </c>
@@ -4502,11 +4521,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A141:A155"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="A73:A87"/>
-    <mergeCell ref="A124:A138"/>
-    <mergeCell ref="A90:A104"/>
     <mergeCell ref="A39:A53"/>
     <mergeCell ref="A56:A70"/>
     <mergeCell ref="C5:D5"/>
@@ -4515,6 +4529,11 @@
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A8:A16"/>
     <mergeCell ref="A19:A36"/>
+    <mergeCell ref="A141:A155"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="A73:A87"/>
+    <mergeCell ref="A124:A138"/>
+    <mergeCell ref="A90:A104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4546,13 +4565,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="178" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
       <c r="F1" s="7"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4582,18 +4601,18 @@
         <v>8</v>
       </c>
       <c r="B3" s="36"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="161"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
     </row>
     <row r="4" spans="1:8" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A4" s="46" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:8" hidden="1" outlineLevel="2">
@@ -4745,9 +4764,9 @@
         <v>9</v>
       </c>
       <c r="B21" s="90"/>
-      <c r="C21" s="164"/>
-      <c r="D21" s="165"/>
-      <c r="E21" s="165"/>
+      <c r="C21" s="162"/>
+      <c r="D21" s="163"/>
+      <c r="E21" s="163"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A22" s="47">
@@ -4898,9 +4917,9 @@
         <v>10</v>
       </c>
       <c r="B38" s="87"/>
-      <c r="C38" s="162"/>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163"/>
+      <c r="C38" s="160"/>
+      <c r="D38" s="161"/>
+      <c r="E38" s="161"/>
     </row>
     <row r="39" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A39" s="47">
@@ -5051,9 +5070,9 @@
         <v>11</v>
       </c>
       <c r="B55" s="87"/>
-      <c r="C55" s="162"/>
-      <c r="D55" s="163"/>
-      <c r="E55" s="163"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="161"/>
+      <c r="E55" s="161"/>
     </row>
     <row r="56" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A56" s="47">
@@ -5204,9 +5223,9 @@
         <v>12</v>
       </c>
       <c r="B72" s="87"/>
-      <c r="C72" s="162"/>
-      <c r="D72" s="163"/>
-      <c r="E72" s="163"/>
+      <c r="C72" s="160"/>
+      <c r="D72" s="161"/>
+      <c r="E72" s="161"/>
     </row>
     <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
@@ -5357,9 +5376,9 @@
         <v>13</v>
       </c>
       <c r="B89" s="87"/>
-      <c r="C89" s="162"/>
-      <c r="D89" s="163"/>
-      <c r="E89" s="163"/>
+      <c r="C89" s="160"/>
+      <c r="D89" s="161"/>
+      <c r="E89" s="161"/>
     </row>
     <row r="90" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A90" s="47">
@@ -5510,9 +5529,9 @@
         <v>14</v>
       </c>
       <c r="B106" s="87"/>
-      <c r="C106" s="162"/>
-      <c r="D106" s="163"/>
-      <c r="E106" s="163"/>
+      <c r="C106" s="160"/>
+      <c r="D106" s="161"/>
+      <c r="E106" s="161"/>
     </row>
     <row r="107" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A107" s="47">
@@ -5663,9 +5682,9 @@
         <v>15</v>
       </c>
       <c r="B123" s="87"/>
-      <c r="C123" s="162"/>
-      <c r="D123" s="163"/>
-      <c r="E123" s="163"/>
+      <c r="C123" s="160"/>
+      <c r="D123" s="161"/>
+      <c r="E123" s="161"/>
     </row>
     <row r="124" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A124" s="47">
@@ -5816,9 +5835,9 @@
         <v>16</v>
       </c>
       <c r="B140" s="87"/>
-      <c r="C140" s="162"/>
-      <c r="D140" s="163"/>
-      <c r="E140" s="163"/>
+      <c r="C140" s="160"/>
+      <c r="D140" s="161"/>
+      <c r="E140" s="161"/>
     </row>
     <row r="141" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A141" s="47">
@@ -5969,9 +5988,9 @@
         <v>17</v>
       </c>
       <c r="B157" s="87"/>
-      <c r="C157" s="162"/>
-      <c r="D157" s="163"/>
-      <c r="E157" s="163"/>
+      <c r="C157" s="160"/>
+      <c r="D157" s="161"/>
+      <c r="E157" s="161"/>
     </row>
     <row r="158" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A158" s="47">
@@ -6122,9 +6141,9 @@
         <v>18</v>
       </c>
       <c r="B174" s="87"/>
-      <c r="C174" s="162"/>
-      <c r="D174" s="163"/>
-      <c r="E174" s="163"/>
+      <c r="C174" s="160"/>
+      <c r="D174" s="161"/>
+      <c r="E174" s="161"/>
     </row>
     <row r="175" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A175" s="47">
@@ -6275,9 +6294,9 @@
         <v>19</v>
       </c>
       <c r="B191" s="87"/>
-      <c r="C191" s="162"/>
-      <c r="D191" s="163"/>
-      <c r="E191" s="163"/>
+      <c r="C191" s="160"/>
+      <c r="D191" s="161"/>
+      <c r="E191" s="161"/>
     </row>
     <row r="192" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A192" s="47">
@@ -6428,9 +6447,9 @@
         <v>20</v>
       </c>
       <c r="B208" s="87"/>
-      <c r="C208" s="162"/>
-      <c r="D208" s="163"/>
-      <c r="E208" s="163"/>
+      <c r="C208" s="160"/>
+      <c r="D208" s="161"/>
+      <c r="E208" s="161"/>
     </row>
     <row r="209" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A209" s="47">
@@ -6581,9 +6600,9 @@
         <v>21</v>
       </c>
       <c r="B225" s="87"/>
-      <c r="C225" s="162"/>
-      <c r="D225" s="163"/>
-      <c r="E225" s="163"/>
+      <c r="C225" s="160"/>
+      <c r="D225" s="161"/>
+      <c r="E225" s="161"/>
     </row>
     <row r="226" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A226" s="47">
@@ -6734,9 +6753,9 @@
         <v>22</v>
       </c>
       <c r="B242" s="87"/>
-      <c r="C242" s="162"/>
-      <c r="D242" s="163"/>
-      <c r="E242" s="163"/>
+      <c r="C242" s="160"/>
+      <c r="D242" s="161"/>
+      <c r="E242" s="161"/>
     </row>
     <row r="243" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A243" s="47">
@@ -6887,9 +6906,9 @@
         <v>23</v>
       </c>
       <c r="B259" s="87"/>
-      <c r="C259" s="162"/>
-      <c r="D259" s="163"/>
-      <c r="E259" s="163"/>
+      <c r="C259" s="160"/>
+      <c r="D259" s="161"/>
+      <c r="E259" s="161"/>
     </row>
     <row r="260" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A260" s="47">
@@ -7040,18 +7059,18 @@
         <v>24</v>
       </c>
       <c r="B276" s="37"/>
-      <c r="C276" s="166"/>
-      <c r="D276" s="167"/>
-      <c r="E276" s="167"/>
+      <c r="C276" s="176"/>
+      <c r="D276" s="177"/>
+      <c r="E276" s="177"/>
     </row>
     <row r="277" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A277" s="51" t="s">
         <v>25</v>
       </c>
       <c r="B277" s="87"/>
-      <c r="C277" s="162"/>
-      <c r="D277" s="163"/>
-      <c r="E277" s="163"/>
+      <c r="C277" s="160"/>
+      <c r="D277" s="161"/>
+      <c r="E277" s="161"/>
     </row>
     <row r="278" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A278" s="52">
@@ -7202,9 +7221,9 @@
         <v>26</v>
       </c>
       <c r="B294" s="90"/>
-      <c r="C294" s="164"/>
-      <c r="D294" s="165"/>
-      <c r="E294" s="165"/>
+      <c r="C294" s="162"/>
+      <c r="D294" s="163"/>
+      <c r="E294" s="163"/>
     </row>
     <row r="295" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A295" s="52">
@@ -7355,9 +7374,9 @@
         <v>27</v>
       </c>
       <c r="B311" s="87"/>
-      <c r="C311" s="162"/>
-      <c r="D311" s="163"/>
-      <c r="E311" s="163"/>
+      <c r="C311" s="160"/>
+      <c r="D311" s="161"/>
+      <c r="E311" s="161"/>
     </row>
     <row r="312" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A312" s="52">
@@ -7508,9 +7527,9 @@
         <v>28</v>
       </c>
       <c r="B328" s="87"/>
-      <c r="C328" s="162"/>
-      <c r="D328" s="163"/>
-      <c r="E328" s="163"/>
+      <c r="C328" s="160"/>
+      <c r="D328" s="161"/>
+      <c r="E328" s="161"/>
     </row>
     <row r="329" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A329" s="52">
@@ -7661,9 +7680,9 @@
         <v>29</v>
       </c>
       <c r="B345" s="87"/>
-      <c r="C345" s="162"/>
-      <c r="D345" s="163"/>
-      <c r="E345" s="163"/>
+      <c r="C345" s="160"/>
+      <c r="D345" s="161"/>
+      <c r="E345" s="161"/>
     </row>
     <row r="346" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A346" s="52">
@@ -7814,9 +7833,9 @@
         <v>30</v>
       </c>
       <c r="B362" s="87"/>
-      <c r="C362" s="162"/>
-      <c r="D362" s="163"/>
-      <c r="E362" s="163"/>
+      <c r="C362" s="160"/>
+      <c r="D362" s="161"/>
+      <c r="E362" s="161"/>
     </row>
     <row r="363" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A363" s="52">
@@ -7967,9 +7986,9 @@
         <v>31</v>
       </c>
       <c r="B379" s="87"/>
-      <c r="C379" s="162"/>
-      <c r="D379" s="163"/>
-      <c r="E379" s="163"/>
+      <c r="C379" s="160"/>
+      <c r="D379" s="161"/>
+      <c r="E379" s="161"/>
     </row>
     <row r="380" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A380" s="52">
@@ -8120,9 +8139,9 @@
         <v>32</v>
       </c>
       <c r="B396" s="87"/>
-      <c r="C396" s="162"/>
-      <c r="D396" s="163"/>
-      <c r="E396" s="163"/>
+      <c r="C396" s="160"/>
+      <c r="D396" s="161"/>
+      <c r="E396" s="161"/>
     </row>
     <row r="397" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A397" s="52">
@@ -8273,9 +8292,9 @@
         <v>33</v>
       </c>
       <c r="B413" s="87"/>
-      <c r="C413" s="162"/>
-      <c r="D413" s="163"/>
-      <c r="E413" s="163"/>
+      <c r="C413" s="160"/>
+      <c r="D413" s="161"/>
+      <c r="E413" s="161"/>
     </row>
     <row r="414" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A414" s="52">
@@ -8426,9 +8445,9 @@
         <v>34</v>
       </c>
       <c r="B430" s="87"/>
-      <c r="C430" s="162"/>
-      <c r="D430" s="163"/>
-      <c r="E430" s="163"/>
+      <c r="C430" s="160"/>
+      <c r="D430" s="161"/>
+      <c r="E430" s="161"/>
     </row>
     <row r="431" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A431" s="52">
@@ -8579,9 +8598,9 @@
         <v>35</v>
       </c>
       <c r="B447" s="87"/>
-      <c r="C447" s="162"/>
-      <c r="D447" s="163"/>
-      <c r="E447" s="163"/>
+      <c r="C447" s="160"/>
+      <c r="D447" s="161"/>
+      <c r="E447" s="161"/>
     </row>
     <row r="448" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A448" s="52">
@@ -8732,9 +8751,9 @@
         <v>36</v>
       </c>
       <c r="B464" s="87"/>
-      <c r="C464" s="162"/>
-      <c r="D464" s="163"/>
-      <c r="E464" s="163"/>
+      <c r="C464" s="160"/>
+      <c r="D464" s="161"/>
+      <c r="E464" s="161"/>
     </row>
     <row r="465" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A465" s="52">
@@ -8885,9 +8904,9 @@
         <v>37</v>
       </c>
       <c r="B481" s="87"/>
-      <c r="C481" s="162"/>
-      <c r="D481" s="163"/>
-      <c r="E481" s="163"/>
+      <c r="C481" s="160"/>
+      <c r="D481" s="161"/>
+      <c r="E481" s="161"/>
     </row>
     <row r="482" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A482" s="52">
@@ -9038,9 +9057,9 @@
         <v>38</v>
       </c>
       <c r="B498" s="87"/>
-      <c r="C498" s="162"/>
-      <c r="D498" s="163"/>
-      <c r="E498" s="163"/>
+      <c r="C498" s="160"/>
+      <c r="D498" s="161"/>
+      <c r="E498" s="161"/>
     </row>
     <row r="499" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A499" s="52">
@@ -9191,9 +9210,9 @@
         <v>39</v>
       </c>
       <c r="B515" s="87"/>
-      <c r="C515" s="162"/>
-      <c r="D515" s="163"/>
-      <c r="E515" s="163"/>
+      <c r="C515" s="160"/>
+      <c r="D515" s="161"/>
+      <c r="E515" s="161"/>
     </row>
     <row r="516" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A516" s="52">
@@ -9344,9 +9363,9 @@
         <v>40</v>
       </c>
       <c r="B532" s="87"/>
-      <c r="C532" s="162"/>
-      <c r="D532" s="163"/>
-      <c r="E532" s="163"/>
+      <c r="C532" s="160"/>
+      <c r="D532" s="161"/>
+      <c r="E532" s="161"/>
     </row>
     <row r="533" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A533" s="55">
@@ -9497,18 +9516,18 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="168"/>
-      <c r="D549" s="169"/>
-      <c r="E549" s="169"/>
+      <c r="C549" s="174"/>
+      <c r="D549" s="175"/>
+      <c r="E549" s="175"/>
     </row>
     <row r="550" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A550" s="58" t="s">
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="162"/>
-      <c r="D550" s="163"/>
-      <c r="E550" s="163"/>
+      <c r="C550" s="160"/>
+      <c r="D550" s="161"/>
+      <c r="E550" s="161"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -9659,9 +9678,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="164"/>
-      <c r="D567" s="165"/>
-      <c r="E567" s="165"/>
+      <c r="C567" s="162"/>
+      <c r="D567" s="163"/>
+      <c r="E567" s="163"/>
     </row>
     <row r="568" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A568" s="59">
@@ -9812,9 +9831,9 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="162"/>
-      <c r="D584" s="163"/>
-      <c r="E584" s="163"/>
+      <c r="C584" s="160"/>
+      <c r="D584" s="161"/>
+      <c r="E584" s="161"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -9965,9 +9984,9 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="162"/>
-      <c r="D601" s="163"/>
-      <c r="E601" s="163"/>
+      <c r="C601" s="160"/>
+      <c r="D601" s="161"/>
+      <c r="E601" s="161"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10118,9 +10137,9 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="162"/>
-      <c r="D618" s="163"/>
-      <c r="E618" s="163"/>
+      <c r="C618" s="160"/>
+      <c r="D618" s="161"/>
+      <c r="E618" s="161"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10271,9 +10290,9 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="162"/>
-      <c r="D635" s="163"/>
-      <c r="E635" s="163"/>
+      <c r="C635" s="160"/>
+      <c r="D635" s="161"/>
+      <c r="E635" s="161"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10424,9 +10443,9 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="162"/>
-      <c r="D652" s="163"/>
-      <c r="E652" s="163"/>
+      <c r="C652" s="160"/>
+      <c r="D652" s="161"/>
+      <c r="E652" s="161"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -10577,9 +10596,9 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="162"/>
-      <c r="D669" s="163"/>
-      <c r="E669" s="163"/>
+      <c r="C669" s="160"/>
+      <c r="D669" s="161"/>
+      <c r="E669" s="161"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -10730,9 +10749,9 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="162"/>
-      <c r="D686" s="163"/>
-      <c r="E686" s="163"/>
+      <c r="C686" s="160"/>
+      <c r="D686" s="161"/>
+      <c r="E686" s="161"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -10883,9 +10902,9 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="162"/>
-      <c r="D703" s="163"/>
-      <c r="E703" s="163"/>
+      <c r="C703" s="160"/>
+      <c r="D703" s="161"/>
+      <c r="E703" s="161"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11036,9 +11055,9 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="162"/>
-      <c r="D720" s="163"/>
-      <c r="E720" s="163"/>
+      <c r="C720" s="160"/>
+      <c r="D720" s="161"/>
+      <c r="E720" s="161"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11189,9 +11208,9 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="162"/>
-      <c r="D737" s="163"/>
-      <c r="E737" s="163"/>
+      <c r="C737" s="160"/>
+      <c r="D737" s="161"/>
+      <c r="E737" s="161"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11342,9 +11361,9 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="162"/>
-      <c r="D754" s="163"/>
-      <c r="E754" s="163"/>
+      <c r="C754" s="160"/>
+      <c r="D754" s="161"/>
+      <c r="E754" s="161"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -11495,9 +11514,9 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="162"/>
-      <c r="D771" s="163"/>
-      <c r="E771" s="163"/>
+      <c r="C771" s="160"/>
+      <c r="D771" s="161"/>
+      <c r="E771" s="161"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -11648,9 +11667,9 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="162"/>
-      <c r="D788" s="163"/>
-      <c r="E788" s="163"/>
+      <c r="C788" s="160"/>
+      <c r="D788" s="161"/>
+      <c r="E788" s="161"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -11801,9 +11820,9 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="162"/>
-      <c r="D805" s="163"/>
-      <c r="E805" s="163"/>
+      <c r="C805" s="160"/>
+      <c r="D805" s="161"/>
+      <c r="E805" s="161"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -11954,18 +11973,18 @@
         <v>67</v>
       </c>
       <c r="B822" s="39"/>
-      <c r="C822" s="170"/>
-      <c r="D822" s="171"/>
-      <c r="E822" s="171"/>
+      <c r="C822" s="172"/>
+      <c r="D822" s="173"/>
+      <c r="E822" s="173"/>
     </row>
     <row r="823" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A823" s="63" t="s">
         <v>68</v>
       </c>
       <c r="B823" s="87"/>
-      <c r="C823" s="162"/>
-      <c r="D823" s="163"/>
-      <c r="E823" s="163"/>
+      <c r="C823" s="160"/>
+      <c r="D823" s="161"/>
+      <c r="E823" s="161"/>
     </row>
     <row r="824" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A824" s="64">
@@ -12116,9 +12135,9 @@
         <v>69</v>
       </c>
       <c r="B840" s="90"/>
-      <c r="C840" s="164"/>
-      <c r="D840" s="165"/>
-      <c r="E840" s="165"/>
+      <c r="C840" s="162"/>
+      <c r="D840" s="163"/>
+      <c r="E840" s="163"/>
     </row>
     <row r="841" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A841" s="64">
@@ -12269,9 +12288,9 @@
         <v>70</v>
       </c>
       <c r="B857" s="87"/>
-      <c r="C857" s="162"/>
-      <c r="D857" s="163"/>
-      <c r="E857" s="163"/>
+      <c r="C857" s="160"/>
+      <c r="D857" s="161"/>
+      <c r="E857" s="161"/>
     </row>
     <row r="858" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A858" s="64">
@@ -12422,9 +12441,9 @@
         <v>71</v>
       </c>
       <c r="B874" s="87"/>
-      <c r="C874" s="162"/>
-      <c r="D874" s="163"/>
-      <c r="E874" s="163"/>
+      <c r="C874" s="160"/>
+      <c r="D874" s="161"/>
+      <c r="E874" s="161"/>
     </row>
     <row r="875" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A875" s="64">
@@ -12575,9 +12594,9 @@
         <v>72</v>
       </c>
       <c r="B891" s="87"/>
-      <c r="C891" s="162"/>
-      <c r="D891" s="163"/>
-      <c r="E891" s="163"/>
+      <c r="C891" s="160"/>
+      <c r="D891" s="161"/>
+      <c r="E891" s="161"/>
     </row>
     <row r="892" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A892" s="64">
@@ -12728,9 +12747,9 @@
         <v>73</v>
       </c>
       <c r="B908" s="87"/>
-      <c r="C908" s="162"/>
-      <c r="D908" s="163"/>
-      <c r="E908" s="163"/>
+      <c r="C908" s="160"/>
+      <c r="D908" s="161"/>
+      <c r="E908" s="161"/>
     </row>
     <row r="909" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A909" s="64">
@@ -12881,9 +12900,9 @@
         <v>74</v>
       </c>
       <c r="B925" s="87"/>
-      <c r="C925" s="162"/>
-      <c r="D925" s="163"/>
-      <c r="E925" s="163"/>
+      <c r="C925" s="160"/>
+      <c r="D925" s="161"/>
+      <c r="E925" s="161"/>
     </row>
     <row r="926" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A926" s="64">
@@ -13034,9 +13053,9 @@
         <v>75</v>
       </c>
       <c r="B942" s="87"/>
-      <c r="C942" s="162"/>
-      <c r="D942" s="163"/>
-      <c r="E942" s="163"/>
+      <c r="C942" s="160"/>
+      <c r="D942" s="161"/>
+      <c r="E942" s="161"/>
     </row>
     <row r="943" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A943" s="64">
@@ -13187,9 +13206,9 @@
         <v>76</v>
       </c>
       <c r="B959" s="87"/>
-      <c r="C959" s="162"/>
-      <c r="D959" s="163"/>
-      <c r="E959" s="163"/>
+      <c r="C959" s="160"/>
+      <c r="D959" s="161"/>
+      <c r="E959" s="161"/>
     </row>
     <row r="960" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A960" s="64">
@@ -13340,9 +13359,9 @@
         <v>77</v>
       </c>
       <c r="B976" s="87"/>
-      <c r="C976" s="162"/>
-      <c r="D976" s="163"/>
-      <c r="E976" s="163"/>
+      <c r="C976" s="160"/>
+      <c r="D976" s="161"/>
+      <c r="E976" s="161"/>
     </row>
     <row r="977" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A977" s="64">
@@ -13493,9 +13512,9 @@
         <v>78</v>
       </c>
       <c r="B993" s="87"/>
-      <c r="C993" s="162"/>
-      <c r="D993" s="163"/>
-      <c r="E993" s="163"/>
+      <c r="C993" s="160"/>
+      <c r="D993" s="161"/>
+      <c r="E993" s="161"/>
     </row>
     <row r="994" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A994" s="64">
@@ -13646,9 +13665,9 @@
         <v>79</v>
       </c>
       <c r="B1010" s="87"/>
-      <c r="C1010" s="162"/>
-      <c r="D1010" s="163"/>
-      <c r="E1010" s="163"/>
+      <c r="C1010" s="160"/>
+      <c r="D1010" s="161"/>
+      <c r="E1010" s="161"/>
     </row>
     <row r="1011" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1011" s="64">
@@ -13799,9 +13818,9 @@
         <v>80</v>
       </c>
       <c r="B1027" s="87"/>
-      <c r="C1027" s="162"/>
-      <c r="D1027" s="163"/>
-      <c r="E1027" s="163"/>
+      <c r="C1027" s="160"/>
+      <c r="D1027" s="161"/>
+      <c r="E1027" s="161"/>
     </row>
     <row r="1028" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1028" s="64">
@@ -13952,9 +13971,9 @@
         <v>83</v>
       </c>
       <c r="B1044" s="87"/>
-      <c r="C1044" s="162"/>
-      <c r="D1044" s="163"/>
-      <c r="E1044" s="163"/>
+      <c r="C1044" s="160"/>
+      <c r="D1044" s="161"/>
+      <c r="E1044" s="161"/>
     </row>
     <row r="1045" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1045" s="64">
@@ -14105,9 +14124,9 @@
         <v>82</v>
       </c>
       <c r="B1061" s="87"/>
-      <c r="C1061" s="162"/>
-      <c r="D1061" s="163"/>
-      <c r="E1061" s="163"/>
+      <c r="C1061" s="160"/>
+      <c r="D1061" s="161"/>
+      <c r="E1061" s="161"/>
     </row>
     <row r="1062" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1062" s="64">
@@ -14258,9 +14277,9 @@
         <v>84</v>
       </c>
       <c r="B1078" s="87"/>
-      <c r="C1078" s="162"/>
-      <c r="D1078" s="163"/>
-      <c r="E1078" s="163"/>
+      <c r="C1078" s="160"/>
+      <c r="D1078" s="161"/>
+      <c r="E1078" s="161"/>
     </row>
     <row r="1079" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1079" s="64">
@@ -14411,18 +14430,18 @@
         <v>104</v>
       </c>
       <c r="B1095" s="40"/>
-      <c r="C1095" s="172"/>
-      <c r="D1095" s="173"/>
-      <c r="E1095" s="173"/>
+      <c r="C1095" s="170"/>
+      <c r="D1095" s="171"/>
+      <c r="E1095" s="171"/>
     </row>
     <row r="1096" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1096" s="68" t="s">
         <v>85</v>
       </c>
       <c r="B1096" s="87"/>
-      <c r="C1096" s="162"/>
-      <c r="D1096" s="163"/>
-      <c r="E1096" s="163"/>
+      <c r="C1096" s="160"/>
+      <c r="D1096" s="161"/>
+      <c r="E1096" s="161"/>
     </row>
     <row r="1097" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1097" s="69">
@@ -14573,9 +14592,9 @@
         <v>86</v>
       </c>
       <c r="B1113" s="90"/>
-      <c r="C1113" s="164"/>
-      <c r="D1113" s="165"/>
-      <c r="E1113" s="165"/>
+      <c r="C1113" s="162"/>
+      <c r="D1113" s="163"/>
+      <c r="E1113" s="163"/>
     </row>
     <row r="1114" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1114" s="69">
@@ -14726,9 +14745,9 @@
         <v>87</v>
       </c>
       <c r="B1130" s="87"/>
-      <c r="C1130" s="162"/>
-      <c r="D1130" s="163"/>
-      <c r="E1130" s="163"/>
+      <c r="C1130" s="160"/>
+      <c r="D1130" s="161"/>
+      <c r="E1130" s="161"/>
     </row>
     <row r="1131" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1131" s="69">
@@ -14879,9 +14898,9 @@
         <v>88</v>
       </c>
       <c r="B1147" s="87"/>
-      <c r="C1147" s="162"/>
-      <c r="D1147" s="163"/>
-      <c r="E1147" s="163"/>
+      <c r="C1147" s="160"/>
+      <c r="D1147" s="161"/>
+      <c r="E1147" s="161"/>
     </row>
     <row r="1148" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1148" s="69">
@@ -15032,9 +15051,9 @@
         <v>89</v>
       </c>
       <c r="B1164" s="87"/>
-      <c r="C1164" s="162"/>
-      <c r="D1164" s="163"/>
-      <c r="E1164" s="163"/>
+      <c r="C1164" s="160"/>
+      <c r="D1164" s="161"/>
+      <c r="E1164" s="161"/>
     </row>
     <row r="1165" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1165" s="69">
@@ -15185,9 +15204,9 @@
         <v>90</v>
       </c>
       <c r="B1181" s="87"/>
-      <c r="C1181" s="162"/>
-      <c r="D1181" s="163"/>
-      <c r="E1181" s="163"/>
+      <c r="C1181" s="160"/>
+      <c r="D1181" s="161"/>
+      <c r="E1181" s="161"/>
     </row>
     <row r="1182" spans="1:5" hidden="1" outlineLevel="3">
       <c r="A1182" s="69">
@@ -15338,9 +15357,9 @@
         <v>91</v>
       </c>
       <c r="B1198" s="87"/>
-      <c r="C1198" s="162"/>
-      <c r="D1198" s="163"/>
-      <c r="E1198" s="163"/>
+      <c r="C1198" s="160"/>
+      <c r="D1198" s="161"/>
+      <c r="E1198" s="161"/>
     </row>
     <row r="1199" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1199" s="69">
@@ -15491,9 +15510,9 @@
         <v>92</v>
       </c>
       <c r="B1215" s="87"/>
-      <c r="C1215" s="162"/>
-      <c r="D1215" s="163"/>
-      <c r="E1215" s="163"/>
+      <c r="C1215" s="160"/>
+      <c r="D1215" s="161"/>
+      <c r="E1215" s="161"/>
     </row>
     <row r="1216" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1216" s="69">
@@ -15644,9 +15663,9 @@
         <v>93</v>
       </c>
       <c r="B1232" s="87"/>
-      <c r="C1232" s="162"/>
-      <c r="D1232" s="163"/>
-      <c r="E1232" s="163"/>
+      <c r="C1232" s="160"/>
+      <c r="D1232" s="161"/>
+      <c r="E1232" s="161"/>
     </row>
     <row r="1233" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1233" s="69">
@@ -15797,9 +15816,9 @@
         <v>94</v>
       </c>
       <c r="B1249" s="87"/>
-      <c r="C1249" s="162"/>
-      <c r="D1249" s="163"/>
-      <c r="E1249" s="163"/>
+      <c r="C1249" s="160"/>
+      <c r="D1249" s="161"/>
+      <c r="E1249" s="161"/>
     </row>
     <row r="1250" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1250" s="69">
@@ -15950,9 +15969,9 @@
         <v>99</v>
       </c>
       <c r="B1266" s="87"/>
-      <c r="C1266" s="162"/>
-      <c r="D1266" s="163"/>
-      <c r="E1266" s="163"/>
+      <c r="C1266" s="160"/>
+      <c r="D1266" s="161"/>
+      <c r="E1266" s="161"/>
     </row>
     <row r="1267" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1267" s="69">
@@ -16103,9 +16122,9 @@
         <v>100</v>
       </c>
       <c r="B1283" s="87"/>
-      <c r="C1283" s="162"/>
-      <c r="D1283" s="163"/>
-      <c r="E1283" s="163"/>
+      <c r="C1283" s="160"/>
+      <c r="D1283" s="161"/>
+      <c r="E1283" s="161"/>
     </row>
     <row r="1284" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1284" s="69">
@@ -16256,9 +16275,9 @@
         <v>101</v>
       </c>
       <c r="B1300" s="87"/>
-      <c r="C1300" s="162"/>
-      <c r="D1300" s="163"/>
-      <c r="E1300" s="163"/>
+      <c r="C1300" s="160"/>
+      <c r="D1300" s="161"/>
+      <c r="E1300" s="161"/>
     </row>
     <row r="1301" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1301" s="69">
@@ -16409,9 +16428,9 @@
         <v>81</v>
       </c>
       <c r="B1317" s="87"/>
-      <c r="C1317" s="162"/>
-      <c r="D1317" s="163"/>
-      <c r="E1317" s="163"/>
+      <c r="C1317" s="160"/>
+      <c r="D1317" s="161"/>
+      <c r="E1317" s="161"/>
     </row>
     <row r="1318" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1318" s="69">
@@ -16562,9 +16581,9 @@
         <v>102</v>
       </c>
       <c r="B1334" s="87"/>
-      <c r="C1334" s="162"/>
-      <c r="D1334" s="163"/>
-      <c r="E1334" s="163"/>
+      <c r="C1334" s="160"/>
+      <c r="D1334" s="161"/>
+      <c r="E1334" s="161"/>
     </row>
     <row r="1335" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1335" s="69">
@@ -16715,9 +16734,9 @@
         <v>98</v>
       </c>
       <c r="B1351" s="87"/>
-      <c r="C1351" s="162"/>
-      <c r="D1351" s="163"/>
-      <c r="E1351" s="163"/>
+      <c r="C1351" s="160"/>
+      <c r="D1351" s="161"/>
+      <c r="E1351" s="161"/>
     </row>
     <row r="1352" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1352" s="69">
@@ -16868,18 +16887,18 @@
         <v>103</v>
       </c>
       <c r="B1368" s="41"/>
-      <c r="C1368" s="174"/>
-      <c r="D1368" s="175"/>
-      <c r="E1368" s="175"/>
+      <c r="C1368" s="168"/>
+      <c r="D1368" s="169"/>
+      <c r="E1368" s="169"/>
     </row>
     <row r="1369" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1369" s="73" t="s">
         <v>105</v>
       </c>
       <c r="B1369" s="87"/>
-      <c r="C1369" s="162"/>
-      <c r="D1369" s="163"/>
-      <c r="E1369" s="163"/>
+      <c r="C1369" s="160"/>
+      <c r="D1369" s="161"/>
+      <c r="E1369" s="161"/>
     </row>
     <row r="1370" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1370" s="74">
@@ -17030,9 +17049,9 @@
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="164"/>
-      <c r="D1386" s="165"/>
-      <c r="E1386" s="165"/>
+      <c r="C1386" s="162"/>
+      <c r="D1386" s="163"/>
+      <c r="E1386" s="163"/>
     </row>
     <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1387" s="74">
@@ -17183,9 +17202,9 @@
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="162"/>
-      <c r="D1403" s="163"/>
-      <c r="E1403" s="163"/>
+      <c r="C1403" s="160"/>
+      <c r="D1403" s="161"/>
+      <c r="E1403" s="161"/>
     </row>
     <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1404" s="74">
@@ -17336,9 +17355,9 @@
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="162"/>
-      <c r="D1420" s="163"/>
-      <c r="E1420" s="163"/>
+      <c r="C1420" s="160"/>
+      <c r="D1420" s="161"/>
+      <c r="E1420" s="161"/>
     </row>
     <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1421" s="74">
@@ -17489,9 +17508,9 @@
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="162"/>
-      <c r="D1437" s="163"/>
-      <c r="E1437" s="163"/>
+      <c r="C1437" s="160"/>
+      <c r="D1437" s="161"/>
+      <c r="E1437" s="161"/>
     </row>
     <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1438" s="74">
@@ -17642,9 +17661,9 @@
         <v>110</v>
       </c>
       <c r="B1454" s="87"/>
-      <c r="C1454" s="162"/>
-      <c r="D1454" s="163"/>
-      <c r="E1454" s="163"/>
+      <c r="C1454" s="160"/>
+      <c r="D1454" s="161"/>
+      <c r="E1454" s="161"/>
     </row>
     <row r="1455" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1455" s="74">
@@ -17795,9 +17814,9 @@
         <v>111</v>
       </c>
       <c r="B1471" s="87"/>
-      <c r="C1471" s="162"/>
-      <c r="D1471" s="163"/>
-      <c r="E1471" s="163"/>
+      <c r="C1471" s="160"/>
+      <c r="D1471" s="161"/>
+      <c r="E1471" s="161"/>
     </row>
     <row r="1472" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1472" s="74">
@@ -17948,9 +17967,9 @@
         <v>112</v>
       </c>
       <c r="B1488" s="87"/>
-      <c r="C1488" s="162"/>
-      <c r="D1488" s="163"/>
-      <c r="E1488" s="163"/>
+      <c r="C1488" s="160"/>
+      <c r="D1488" s="161"/>
+      <c r="E1488" s="161"/>
     </row>
     <row r="1489" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1489" s="74">
@@ -18101,9 +18120,9 @@
         <v>113</v>
       </c>
       <c r="B1505" s="87"/>
-      <c r="C1505" s="162"/>
-      <c r="D1505" s="163"/>
-      <c r="E1505" s="163"/>
+      <c r="C1505" s="160"/>
+      <c r="D1505" s="161"/>
+      <c r="E1505" s="161"/>
     </row>
     <row r="1506" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1506" s="74">
@@ -18254,9 +18273,9 @@
         <v>114</v>
       </c>
       <c r="B1522" s="87"/>
-      <c r="C1522" s="162"/>
-      <c r="D1522" s="163"/>
-      <c r="E1522" s="163"/>
+      <c r="C1522" s="160"/>
+      <c r="D1522" s="161"/>
+      <c r="E1522" s="161"/>
     </row>
     <row r="1523" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1523" s="74">
@@ -18407,9 +18426,9 @@
         <v>95</v>
       </c>
       <c r="B1539" s="87"/>
-      <c r="C1539" s="162"/>
-      <c r="D1539" s="163"/>
-      <c r="E1539" s="163"/>
+      <c r="C1539" s="160"/>
+      <c r="D1539" s="161"/>
+      <c r="E1539" s="161"/>
     </row>
     <row r="1540" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1540" s="74">
@@ -18560,9 +18579,9 @@
         <v>115</v>
       </c>
       <c r="B1556" s="87"/>
-      <c r="C1556" s="162"/>
-      <c r="D1556" s="163"/>
-      <c r="E1556" s="163"/>
+      <c r="C1556" s="160"/>
+      <c r="D1556" s="161"/>
+      <c r="E1556" s="161"/>
     </row>
     <row r="1557" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1557" s="74">
@@ -18713,9 +18732,9 @@
         <v>116</v>
       </c>
       <c r="B1573" s="87"/>
-      <c r="C1573" s="162"/>
-      <c r="D1573" s="163"/>
-      <c r="E1573" s="163"/>
+      <c r="C1573" s="160"/>
+      <c r="D1573" s="161"/>
+      <c r="E1573" s="161"/>
     </row>
     <row r="1574" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1574" s="74">
@@ -18866,9 +18885,9 @@
         <v>117</v>
       </c>
       <c r="B1590" s="87"/>
-      <c r="C1590" s="162"/>
-      <c r="D1590" s="163"/>
-      <c r="E1590" s="163"/>
+      <c r="C1590" s="160"/>
+      <c r="D1590" s="161"/>
+      <c r="E1590" s="161"/>
     </row>
     <row r="1591" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1591" s="74">
@@ -19019,9 +19038,9 @@
         <v>118</v>
       </c>
       <c r="B1607" s="87"/>
-      <c r="C1607" s="162"/>
-      <c r="D1607" s="163"/>
-      <c r="E1607" s="163"/>
+      <c r="C1607" s="160"/>
+      <c r="D1607" s="161"/>
+      <c r="E1607" s="161"/>
     </row>
     <row r="1608" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1608" s="74">
@@ -19172,9 +19191,9 @@
         <v>119</v>
       </c>
       <c r="B1624" s="87"/>
-      <c r="C1624" s="162"/>
-      <c r="D1624" s="163"/>
-      <c r="E1624" s="163"/>
+      <c r="C1624" s="160"/>
+      <c r="D1624" s="161"/>
+      <c r="E1624" s="161"/>
     </row>
     <row r="1625" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1625" s="74">
@@ -19325,18 +19344,18 @@
         <v>120</v>
       </c>
       <c r="B1641" s="42"/>
-      <c r="C1641" s="176"/>
-      <c r="D1641" s="177"/>
-      <c r="E1641" s="177"/>
+      <c r="C1641" s="166"/>
+      <c r="D1641" s="167"/>
+      <c r="E1641" s="167"/>
     </row>
     <row r="1642" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1642" s="78" t="s">
         <v>121</v>
       </c>
       <c r="B1642" s="87"/>
-      <c r="C1642" s="162"/>
-      <c r="D1642" s="163"/>
-      <c r="E1642" s="163"/>
+      <c r="C1642" s="160"/>
+      <c r="D1642" s="161"/>
+      <c r="E1642" s="161"/>
     </row>
     <row r="1643" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1643" s="79">
@@ -19487,9 +19506,9 @@
         <v>122</v>
       </c>
       <c r="B1659" s="90"/>
-      <c r="C1659" s="164"/>
-      <c r="D1659" s="165"/>
-      <c r="E1659" s="165"/>
+      <c r="C1659" s="162"/>
+      <c r="D1659" s="163"/>
+      <c r="E1659" s="163"/>
     </row>
     <row r="1660" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1660" s="79">
@@ -19640,9 +19659,9 @@
         <v>123</v>
       </c>
       <c r="B1676" s="87"/>
-      <c r="C1676" s="162"/>
-      <c r="D1676" s="163"/>
-      <c r="E1676" s="163"/>
+      <c r="C1676" s="160"/>
+      <c r="D1676" s="161"/>
+      <c r="E1676" s="161"/>
     </row>
     <row r="1677" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1677" s="79">
@@ -19793,9 +19812,9 @@
         <v>124</v>
       </c>
       <c r="B1693" s="87"/>
-      <c r="C1693" s="162"/>
-      <c r="D1693" s="163"/>
-      <c r="E1693" s="163"/>
+      <c r="C1693" s="160"/>
+      <c r="D1693" s="161"/>
+      <c r="E1693" s="161"/>
     </row>
     <row r="1694" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1694" s="79">
@@ -19946,9 +19965,9 @@
         <v>125</v>
       </c>
       <c r="B1710" s="87"/>
-      <c r="C1710" s="162"/>
-      <c r="D1710" s="163"/>
-      <c r="E1710" s="163"/>
+      <c r="C1710" s="160"/>
+      <c r="D1710" s="161"/>
+      <c r="E1710" s="161"/>
     </row>
     <row r="1711" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1711" s="79">
@@ -20099,9 +20118,9 @@
         <v>126</v>
       </c>
       <c r="B1727" s="87"/>
-      <c r="C1727" s="162"/>
-      <c r="D1727" s="163"/>
-      <c r="E1727" s="163"/>
+      <c r="C1727" s="160"/>
+      <c r="D1727" s="161"/>
+      <c r="E1727" s="161"/>
     </row>
     <row r="1728" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1728" s="79">
@@ -20252,9 +20271,9 @@
         <v>127</v>
       </c>
       <c r="B1744" s="87"/>
-      <c r="C1744" s="162"/>
-      <c r="D1744" s="163"/>
-      <c r="E1744" s="163"/>
+      <c r="C1744" s="160"/>
+      <c r="D1744" s="161"/>
+      <c r="E1744" s="161"/>
     </row>
     <row r="1745" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1745" s="79">
@@ -20405,9 +20424,9 @@
         <v>128</v>
       </c>
       <c r="B1761" s="87"/>
-      <c r="C1761" s="162"/>
-      <c r="D1761" s="163"/>
-      <c r="E1761" s="163"/>
+      <c r="C1761" s="160"/>
+      <c r="D1761" s="161"/>
+      <c r="E1761" s="161"/>
     </row>
     <row r="1762" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1762" s="79">
@@ -20558,9 +20577,9 @@
         <v>129</v>
       </c>
       <c r="B1778" s="87"/>
-      <c r="C1778" s="162"/>
-      <c r="D1778" s="163"/>
-      <c r="E1778" s="163"/>
+      <c r="C1778" s="160"/>
+      <c r="D1778" s="161"/>
+      <c r="E1778" s="161"/>
     </row>
     <row r="1779" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1779" s="79">
@@ -20711,9 +20730,9 @@
         <v>130</v>
       </c>
       <c r="B1795" s="87"/>
-      <c r="C1795" s="162"/>
-      <c r="D1795" s="163"/>
-      <c r="E1795" s="163"/>
+      <c r="C1795" s="160"/>
+      <c r="D1795" s="161"/>
+      <c r="E1795" s="161"/>
     </row>
     <row r="1796" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1796" s="79">
@@ -20864,9 +20883,9 @@
         <v>131</v>
       </c>
       <c r="B1812" s="87"/>
-      <c r="C1812" s="162"/>
-      <c r="D1812" s="163"/>
-      <c r="E1812" s="163"/>
+      <c r="C1812" s="160"/>
+      <c r="D1812" s="161"/>
+      <c r="E1812" s="161"/>
     </row>
     <row r="1813" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1813" s="79">
@@ -21017,9 +21036,9 @@
         <v>96</v>
       </c>
       <c r="B1829" s="87"/>
-      <c r="C1829" s="162"/>
-      <c r="D1829" s="163"/>
-      <c r="E1829" s="163"/>
+      <c r="C1829" s="160"/>
+      <c r="D1829" s="161"/>
+      <c r="E1829" s="161"/>
     </row>
     <row r="1830" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1830" s="79">
@@ -21170,9 +21189,9 @@
         <v>132</v>
       </c>
       <c r="B1846" s="87"/>
-      <c r="C1846" s="162"/>
-      <c r="D1846" s="163"/>
-      <c r="E1846" s="163"/>
+      <c r="C1846" s="160"/>
+      <c r="D1846" s="161"/>
+      <c r="E1846" s="161"/>
     </row>
     <row r="1847" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1847" s="79">
@@ -21323,9 +21342,9 @@
         <v>133</v>
       </c>
       <c r="B1863" s="87"/>
-      <c r="C1863" s="162"/>
-      <c r="D1863" s="163"/>
-      <c r="E1863" s="163"/>
+      <c r="C1863" s="160"/>
+      <c r="D1863" s="161"/>
+      <c r="E1863" s="161"/>
     </row>
     <row r="1864" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1864" s="79">
@@ -21476,9 +21495,9 @@
         <v>134</v>
       </c>
       <c r="B1880" s="87"/>
-      <c r="C1880" s="162"/>
-      <c r="D1880" s="163"/>
-      <c r="E1880" s="163"/>
+      <c r="C1880" s="160"/>
+      <c r="D1880" s="161"/>
+      <c r="E1880" s="161"/>
     </row>
     <row r="1881" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1881" s="79">
@@ -21629,9 +21648,9 @@
         <v>135</v>
       </c>
       <c r="B1897" s="87"/>
-      <c r="C1897" s="162"/>
-      <c r="D1897" s="163"/>
-      <c r="E1897" s="163"/>
+      <c r="C1897" s="160"/>
+      <c r="D1897" s="161"/>
+      <c r="E1897" s="161"/>
     </row>
     <row r="1898" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1898" s="79">
@@ -21782,18 +21801,18 @@
         <v>136</v>
       </c>
       <c r="B1914" s="43"/>
-      <c r="C1914" s="178"/>
-      <c r="D1914" s="179"/>
-      <c r="E1914" s="179"/>
+      <c r="C1914" s="164"/>
+      <c r="D1914" s="165"/>
+      <c r="E1914" s="165"/>
     </row>
     <row r="1915" spans="1:5" ht="18" hidden="1" outlineLevel="1" collapsed="1">
       <c r="A1915" s="83" t="s">
         <v>137</v>
       </c>
       <c r="B1915" s="87"/>
-      <c r="C1915" s="162"/>
-      <c r="D1915" s="163"/>
-      <c r="E1915" s="163"/>
+      <c r="C1915" s="160"/>
+      <c r="D1915" s="161"/>
+      <c r="E1915" s="161"/>
     </row>
     <row r="1916" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1916" s="84">
@@ -21944,9 +21963,9 @@
         <v>138</v>
       </c>
       <c r="B1932" s="90"/>
-      <c r="C1932" s="164"/>
-      <c r="D1932" s="165"/>
-      <c r="E1932" s="165"/>
+      <c r="C1932" s="162"/>
+      <c r="D1932" s="163"/>
+      <c r="E1932" s="163"/>
     </row>
     <row r="1933" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1933" s="84">
@@ -22097,9 +22116,9 @@
         <v>139</v>
       </c>
       <c r="B1949" s="87"/>
-      <c r="C1949" s="162"/>
-      <c r="D1949" s="163"/>
-      <c r="E1949" s="163"/>
+      <c r="C1949" s="160"/>
+      <c r="D1949" s="161"/>
+      <c r="E1949" s="161"/>
     </row>
     <row r="1950" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1950" s="84">
@@ -22250,9 +22269,9 @@
         <v>140</v>
       </c>
       <c r="B1966" s="87"/>
-      <c r="C1966" s="162"/>
-      <c r="D1966" s="163"/>
-      <c r="E1966" s="163"/>
+      <c r="C1966" s="160"/>
+      <c r="D1966" s="161"/>
+      <c r="E1966" s="161"/>
     </row>
     <row r="1967" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1967" s="84">
@@ -22403,9 +22422,9 @@
         <v>141</v>
       </c>
       <c r="B1983" s="87"/>
-      <c r="C1983" s="162"/>
-      <c r="D1983" s="163"/>
-      <c r="E1983" s="163"/>
+      <c r="C1983" s="160"/>
+      <c r="D1983" s="161"/>
+      <c r="E1983" s="161"/>
     </row>
     <row r="1984" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A1984" s="84">
@@ -22556,9 +22575,9 @@
         <v>142</v>
       </c>
       <c r="B2000" s="87"/>
-      <c r="C2000" s="162"/>
-      <c r="D2000" s="163"/>
-      <c r="E2000" s="163"/>
+      <c r="C2000" s="160"/>
+      <c r="D2000" s="161"/>
+      <c r="E2000" s="161"/>
     </row>
     <row r="2001" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2001" s="84">
@@ -22709,9 +22728,9 @@
         <v>143</v>
       </c>
       <c r="B2017" s="87"/>
-      <c r="C2017" s="162"/>
-      <c r="D2017" s="163"/>
-      <c r="E2017" s="163"/>
+      <c r="C2017" s="160"/>
+      <c r="D2017" s="161"/>
+      <c r="E2017" s="161"/>
     </row>
     <row r="2018" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2018" s="84">
@@ -22862,9 +22881,9 @@
         <v>144</v>
       </c>
       <c r="B2034" s="87"/>
-      <c r="C2034" s="162"/>
-      <c r="D2034" s="163"/>
-      <c r="E2034" s="163"/>
+      <c r="C2034" s="160"/>
+      <c r="D2034" s="161"/>
+      <c r="E2034" s="161"/>
     </row>
     <row r="2035" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2035" s="84">
@@ -23015,9 +23034,9 @@
         <v>145</v>
       </c>
       <c r="B2051" s="87"/>
-      <c r="C2051" s="162"/>
-      <c r="D2051" s="163"/>
-      <c r="E2051" s="163"/>
+      <c r="C2051" s="160"/>
+      <c r="D2051" s="161"/>
+      <c r="E2051" s="161"/>
     </row>
     <row r="2052" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2052" s="84">
@@ -23168,9 +23187,9 @@
         <v>146</v>
       </c>
       <c r="B2068" s="87"/>
-      <c r="C2068" s="162"/>
-      <c r="D2068" s="163"/>
-      <c r="E2068" s="163"/>
+      <c r="C2068" s="160"/>
+      <c r="D2068" s="161"/>
+      <c r="E2068" s="161"/>
     </row>
     <row r="2069" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2069" s="84">
@@ -23321,9 +23340,9 @@
         <v>147</v>
       </c>
       <c r="B2085" s="87"/>
-      <c r="C2085" s="162"/>
-      <c r="D2085" s="163"/>
-      <c r="E2085" s="163"/>
+      <c r="C2085" s="160"/>
+      <c r="D2085" s="161"/>
+      <c r="E2085" s="161"/>
     </row>
     <row r="2086" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2086" s="84">
@@ -23474,9 +23493,9 @@
         <v>148</v>
       </c>
       <c r="B2102" s="87"/>
-      <c r="C2102" s="162"/>
-      <c r="D2102" s="163"/>
-      <c r="E2102" s="163"/>
+      <c r="C2102" s="160"/>
+      <c r="D2102" s="161"/>
+      <c r="E2102" s="161"/>
     </row>
     <row r="2103" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2103" s="84">
@@ -23627,9 +23646,9 @@
         <v>97</v>
       </c>
       <c r="B2119" s="87"/>
-      <c r="C2119" s="162"/>
-      <c r="D2119" s="163"/>
-      <c r="E2119" s="163"/>
+      <c r="C2119" s="160"/>
+      <c r="D2119" s="161"/>
+      <c r="E2119" s="161"/>
     </row>
     <row r="2120" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2120" s="84">
@@ -23780,9 +23799,9 @@
         <v>149</v>
       </c>
       <c r="B2136" s="87"/>
-      <c r="C2136" s="162"/>
-      <c r="D2136" s="163"/>
-      <c r="E2136" s="163"/>
+      <c r="C2136" s="160"/>
+      <c r="D2136" s="161"/>
+      <c r="E2136" s="161"/>
     </row>
     <row r="2137" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2137" s="84">
@@ -23933,9 +23952,9 @@
         <v>150</v>
       </c>
       <c r="B2153" s="87"/>
-      <c r="C2153" s="162"/>
-      <c r="D2153" s="163"/>
-      <c r="E2153" s="163"/>
+      <c r="C2153" s="160"/>
+      <c r="D2153" s="161"/>
+      <c r="E2153" s="161"/>
     </row>
     <row r="2154" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2154" s="84">
@@ -24086,9 +24105,9 @@
         <v>151</v>
       </c>
       <c r="B2170" s="87"/>
-      <c r="C2170" s="162"/>
-      <c r="D2170" s="163"/>
-      <c r="E2170" s="163"/>
+      <c r="C2170" s="160"/>
+      <c r="D2170" s="161"/>
+      <c r="E2170" s="161"/>
     </row>
     <row r="2171" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A2171" s="84">
@@ -24236,15 +24255,122 @@
     </row>
   </sheetData>
   <mergeCells count="137">
-    <mergeCell ref="C2034:E2034"/>
-    <mergeCell ref="C2051:E2051"/>
-    <mergeCell ref="C2068:E2068"/>
-    <mergeCell ref="C2085:E2085"/>
-    <mergeCell ref="C2170:E2170"/>
-    <mergeCell ref="C2102:E2102"/>
-    <mergeCell ref="C2119:E2119"/>
-    <mergeCell ref="C2136:E2136"/>
-    <mergeCell ref="C2153:E2153"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C225:E225"/>
+    <mergeCell ref="C242:E242"/>
+    <mergeCell ref="C259:E259"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C157:E157"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="C413:E413"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="C447:E447"/>
+    <mergeCell ref="C464:E464"/>
+    <mergeCell ref="C481:E481"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="C328:E328"/>
+    <mergeCell ref="C345:E345"/>
+    <mergeCell ref="C362:E362"/>
+    <mergeCell ref="C379:E379"/>
+    <mergeCell ref="C584:E584"/>
+    <mergeCell ref="C601:E601"/>
+    <mergeCell ref="C618:E618"/>
+    <mergeCell ref="C635:E635"/>
+    <mergeCell ref="C652:E652"/>
+    <mergeCell ref="C669:E669"/>
+    <mergeCell ref="C498:E498"/>
+    <mergeCell ref="C515:E515"/>
+    <mergeCell ref="C532:E532"/>
+    <mergeCell ref="C549:E549"/>
+    <mergeCell ref="C550:E550"/>
+    <mergeCell ref="C567:E567"/>
+    <mergeCell ref="C788:E788"/>
+    <mergeCell ref="C805:E805"/>
+    <mergeCell ref="C822:E822"/>
+    <mergeCell ref="C823:E823"/>
+    <mergeCell ref="C840:E840"/>
+    <mergeCell ref="C857:E857"/>
+    <mergeCell ref="C686:E686"/>
+    <mergeCell ref="C703:E703"/>
+    <mergeCell ref="C720:E720"/>
+    <mergeCell ref="C737:E737"/>
+    <mergeCell ref="C754:E754"/>
+    <mergeCell ref="C771:E771"/>
+    <mergeCell ref="C976:E976"/>
+    <mergeCell ref="C993:E993"/>
+    <mergeCell ref="C1010:E1010"/>
+    <mergeCell ref="C1027:E1027"/>
+    <mergeCell ref="C1044:E1044"/>
+    <mergeCell ref="C1061:E1061"/>
+    <mergeCell ref="C874:E874"/>
+    <mergeCell ref="C891:E891"/>
+    <mergeCell ref="C908:E908"/>
+    <mergeCell ref="C925:E925"/>
+    <mergeCell ref="C942:E942"/>
+    <mergeCell ref="C959:E959"/>
+    <mergeCell ref="C1164:E1164"/>
+    <mergeCell ref="C1181:E1181"/>
+    <mergeCell ref="C1198:E1198"/>
+    <mergeCell ref="C1215:E1215"/>
+    <mergeCell ref="C1232:E1232"/>
+    <mergeCell ref="C1249:E1249"/>
+    <mergeCell ref="C1078:E1078"/>
+    <mergeCell ref="C1095:E1095"/>
+    <mergeCell ref="C1096:E1096"/>
+    <mergeCell ref="C1113:E1113"/>
+    <mergeCell ref="C1130:E1130"/>
+    <mergeCell ref="C1147:E1147"/>
+    <mergeCell ref="C1368:E1368"/>
+    <mergeCell ref="C1369:E1369"/>
+    <mergeCell ref="C1386:E1386"/>
+    <mergeCell ref="C1403:E1403"/>
+    <mergeCell ref="C1420:E1420"/>
+    <mergeCell ref="C1437:E1437"/>
+    <mergeCell ref="C1266:E1266"/>
+    <mergeCell ref="C1283:E1283"/>
+    <mergeCell ref="C1300:E1300"/>
+    <mergeCell ref="C1317:E1317"/>
+    <mergeCell ref="C1334:E1334"/>
+    <mergeCell ref="C1351:E1351"/>
+    <mergeCell ref="C1556:E1556"/>
+    <mergeCell ref="C1573:E1573"/>
+    <mergeCell ref="C1590:E1590"/>
+    <mergeCell ref="C1607:E1607"/>
+    <mergeCell ref="C1624:E1624"/>
+    <mergeCell ref="C1641:E1641"/>
+    <mergeCell ref="C1454:E1454"/>
+    <mergeCell ref="C1471:E1471"/>
+    <mergeCell ref="C1488:E1488"/>
+    <mergeCell ref="C1505:E1505"/>
+    <mergeCell ref="C1522:E1522"/>
+    <mergeCell ref="C1539:E1539"/>
+    <mergeCell ref="C1744:E1744"/>
+    <mergeCell ref="C1761:E1761"/>
+    <mergeCell ref="C1778:E1778"/>
+    <mergeCell ref="C1795:E1795"/>
+    <mergeCell ref="C1812:E1812"/>
+    <mergeCell ref="C1829:E1829"/>
+    <mergeCell ref="C1642:E1642"/>
+    <mergeCell ref="C1659:E1659"/>
+    <mergeCell ref="C1676:E1676"/>
+    <mergeCell ref="C1693:E1693"/>
+    <mergeCell ref="C1710:E1710"/>
+    <mergeCell ref="C1727:E1727"/>
     <mergeCell ref="C1932:E1932"/>
     <mergeCell ref="C1949:E1949"/>
     <mergeCell ref="C1966:E1966"/>
@@ -24257,124 +24383,17 @@
     <mergeCell ref="C1897:E1897"/>
     <mergeCell ref="C1914:E1914"/>
     <mergeCell ref="C1915:E1915"/>
-    <mergeCell ref="C1744:E1744"/>
-    <mergeCell ref="C1761:E1761"/>
-    <mergeCell ref="C1778:E1778"/>
-    <mergeCell ref="C1795:E1795"/>
-    <mergeCell ref="C1812:E1812"/>
-    <mergeCell ref="C1829:E1829"/>
-    <mergeCell ref="C1642:E1642"/>
-    <mergeCell ref="C1659:E1659"/>
-    <mergeCell ref="C1676:E1676"/>
-    <mergeCell ref="C1693:E1693"/>
-    <mergeCell ref="C1710:E1710"/>
-    <mergeCell ref="C1727:E1727"/>
-    <mergeCell ref="C1556:E1556"/>
-    <mergeCell ref="C1573:E1573"/>
-    <mergeCell ref="C1590:E1590"/>
-    <mergeCell ref="C1607:E1607"/>
-    <mergeCell ref="C1624:E1624"/>
-    <mergeCell ref="C1641:E1641"/>
-    <mergeCell ref="C1454:E1454"/>
-    <mergeCell ref="C1471:E1471"/>
-    <mergeCell ref="C1488:E1488"/>
-    <mergeCell ref="C1505:E1505"/>
-    <mergeCell ref="C1522:E1522"/>
-    <mergeCell ref="C1539:E1539"/>
-    <mergeCell ref="C1368:E1368"/>
-    <mergeCell ref="C1369:E1369"/>
-    <mergeCell ref="C1386:E1386"/>
-    <mergeCell ref="C1403:E1403"/>
-    <mergeCell ref="C1420:E1420"/>
-    <mergeCell ref="C1437:E1437"/>
-    <mergeCell ref="C1266:E1266"/>
-    <mergeCell ref="C1283:E1283"/>
-    <mergeCell ref="C1300:E1300"/>
-    <mergeCell ref="C1317:E1317"/>
-    <mergeCell ref="C1334:E1334"/>
-    <mergeCell ref="C1351:E1351"/>
-    <mergeCell ref="C1164:E1164"/>
-    <mergeCell ref="C1181:E1181"/>
-    <mergeCell ref="C1198:E1198"/>
-    <mergeCell ref="C1215:E1215"/>
-    <mergeCell ref="C1232:E1232"/>
-    <mergeCell ref="C1249:E1249"/>
-    <mergeCell ref="C1078:E1078"/>
-    <mergeCell ref="C1095:E1095"/>
-    <mergeCell ref="C1096:E1096"/>
-    <mergeCell ref="C1113:E1113"/>
-    <mergeCell ref="C1130:E1130"/>
-    <mergeCell ref="C1147:E1147"/>
-    <mergeCell ref="C976:E976"/>
-    <mergeCell ref="C993:E993"/>
-    <mergeCell ref="C1010:E1010"/>
-    <mergeCell ref="C1027:E1027"/>
-    <mergeCell ref="C1044:E1044"/>
-    <mergeCell ref="C1061:E1061"/>
-    <mergeCell ref="C874:E874"/>
-    <mergeCell ref="C891:E891"/>
-    <mergeCell ref="C908:E908"/>
-    <mergeCell ref="C925:E925"/>
-    <mergeCell ref="C942:E942"/>
-    <mergeCell ref="C959:E959"/>
-    <mergeCell ref="C788:E788"/>
-    <mergeCell ref="C805:E805"/>
-    <mergeCell ref="C822:E822"/>
-    <mergeCell ref="C823:E823"/>
-    <mergeCell ref="C840:E840"/>
-    <mergeCell ref="C857:E857"/>
-    <mergeCell ref="C686:E686"/>
-    <mergeCell ref="C703:E703"/>
-    <mergeCell ref="C720:E720"/>
-    <mergeCell ref="C737:E737"/>
-    <mergeCell ref="C754:E754"/>
-    <mergeCell ref="C771:E771"/>
-    <mergeCell ref="C584:E584"/>
-    <mergeCell ref="C601:E601"/>
-    <mergeCell ref="C618:E618"/>
-    <mergeCell ref="C635:E635"/>
-    <mergeCell ref="C652:E652"/>
-    <mergeCell ref="C669:E669"/>
-    <mergeCell ref="C498:E498"/>
-    <mergeCell ref="C515:E515"/>
-    <mergeCell ref="C532:E532"/>
-    <mergeCell ref="C549:E549"/>
-    <mergeCell ref="C550:E550"/>
-    <mergeCell ref="C567:E567"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="C413:E413"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="C447:E447"/>
-    <mergeCell ref="C464:E464"/>
-    <mergeCell ref="C481:E481"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="C328:E328"/>
-    <mergeCell ref="C345:E345"/>
-    <mergeCell ref="C362:E362"/>
-    <mergeCell ref="C379:E379"/>
-    <mergeCell ref="C225:E225"/>
-    <mergeCell ref="C242:E242"/>
-    <mergeCell ref="C259:E259"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C157:E157"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C2034:E2034"/>
+    <mergeCell ref="C2051:E2051"/>
+    <mergeCell ref="C2068:E2068"/>
+    <mergeCell ref="C2085:E2085"/>
+    <mergeCell ref="C2170:E2170"/>
+    <mergeCell ref="C2102:E2102"/>
+    <mergeCell ref="C2119:E2119"/>
+    <mergeCell ref="C2136:E2136"/>
+    <mergeCell ref="C2153:E2153"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24399,51 +24418,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" thickBot="1">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="186"/>
-      <c r="C1" s="186"/>
-      <c r="D1" s="186"/>
-      <c r="E1" s="186"/>
-      <c r="F1" s="186"/>
-      <c r="G1" s="186"/>
-      <c r="H1" s="186"/>
-      <c r="I1" s="186"/>
-      <c r="J1" s="186"/>
-      <c r="K1" s="186"/>
-      <c r="L1" s="186"/>
+      <c r="B1" s="187"/>
+      <c r="C1" s="187"/>
+      <c r="D1" s="187"/>
+      <c r="E1" s="187"/>
+      <c r="F1" s="187"/>
+      <c r="G1" s="187"/>
+      <c r="H1" s="187"/>
+      <c r="I1" s="187"/>
+      <c r="J1" s="187"/>
+      <c r="K1" s="187"/>
+      <c r="L1" s="187"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" thickBot="1">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="184" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
-      <c r="H2" s="184"/>
-      <c r="I2" s="184"/>
-      <c r="J2" s="184"/>
-      <c r="K2" s="184"/>
-      <c r="L2" s="185"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="185"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="185"/>
+      <c r="I2" s="185"/>
+      <c r="J2" s="185"/>
+      <c r="K2" s="185"/>
+      <c r="L2" s="186"/>
     </row>
     <row r="3" spans="1:12" s="31" customFormat="1" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="181" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="182"/>
+      <c r="B3" s="182"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="182"/>
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="182"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="183"/>
     </row>
     <row r="4" spans="1:12" s="27" customFormat="1">
       <c r="A4" s="28" t="s">
@@ -24660,19 +24679,19 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A20" s="180" t="s">
+      <c r="A20" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="181"/>
-      <c r="C20" s="181"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="182"/>
+      <c r="D20" s="182"/>
+      <c r="E20" s="182"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="182"/>
+      <c r="I20" s="182"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="183"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="28" t="s">
@@ -24889,19 +24908,19 @@
       <c r="K36" s="2"/>
     </row>
     <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A37" s="180" t="s">
+      <c r="A37" s="181" t="s">
         <v>167</v>
       </c>
-      <c r="B37" s="181"/>
-      <c r="C37" s="181"/>
-      <c r="D37" s="181"/>
-      <c r="E37" s="181"/>
-      <c r="F37" s="181"/>
-      <c r="G37" s="181"/>
-      <c r="H37" s="181"/>
-      <c r="I37" s="181"/>
-      <c r="J37" s="181"/>
-      <c r="K37" s="182"/>
+      <c r="B37" s="182"/>
+      <c r="C37" s="182"/>
+      <c r="D37" s="182"/>
+      <c r="E37" s="182"/>
+      <c r="F37" s="182"/>
+      <c r="G37" s="182"/>
+      <c r="H37" s="182"/>
+      <c r="I37" s="182"/>
+      <c r="J37" s="182"/>
+      <c r="K37" s="183"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="28" t="s">
@@ -25125,7 +25144,7 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A20:K20"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25159,28 +25178,28 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="187"/>
+      <c r="A3" s="188"/>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="188"/>
+      <c r="A4" s="189"/>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="188"/>
+      <c r="A5" s="189"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="188"/>
+      <c r="A6" s="189"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="188"/>
+      <c r="A7" s="189"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="188"/>
+      <c r="A8" s="189"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="188"/>
+      <c r="A9" s="189"/>
     </row>
     <row r="10" spans="1:1" ht="13.5" thickBot="1">
-      <c r="A10" s="189"/>
+      <c r="A10" s="190"/>
     </row>
     <row r="11" spans="1:1" ht="27" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -25336,7 +25355,7 @@
   <mergeCells count="1">
     <mergeCell ref="A3:A10"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -25363,10 +25382,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B1" s="190" t="s">
+      <c r="B1" s="191" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="191"/>
+      <c r="C1" s="192"/>
       <c r="D1" s="92"/>
       <c r="E1" s="32"/>
     </row>
@@ -25377,7 +25396,7 @@
       <c r="E2" s="119"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="193" t="s">
         <v>208</v>
       </c>
       <c r="B3" s="131" t="s">
@@ -25391,7 +25410,7 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="193"/>
+      <c r="A4" s="194"/>
       <c r="B4" s="128" t="s">
         <v>159</v>
       </c>
@@ -25403,7 +25422,7 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="193"/>
+      <c r="A5" s="194"/>
       <c r="B5" s="128" t="s">
         <v>160</v>
       </c>
@@ -25412,7 +25431,7 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="193"/>
+      <c r="A6" s="194"/>
       <c r="B6" s="139" t="s">
         <v>210</v>
       </c>
@@ -25424,7 +25443,7 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="193"/>
+      <c r="A7" s="194"/>
       <c r="B7" s="128" t="s">
         <v>177</v>
       </c>
@@ -25436,7 +25455,7 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="193"/>
+      <c r="A8" s="194"/>
       <c r="B8" s="128" t="s">
         <v>178</v>
       </c>
@@ -25445,7 +25464,7 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A9" s="194"/>
+      <c r="A9" s="195"/>
       <c r="B9" s="136" t="s">
         <v>161</v>
       </c>
@@ -25460,7 +25479,7 @@
       <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A11" s="192" t="s">
+      <c r="A11" s="193" t="s">
         <v>209</v>
       </c>
       <c r="B11" s="131" t="s">
@@ -25474,7 +25493,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="193"/>
+      <c r="A12" s="194"/>
       <c r="B12" s="128" t="s">
         <v>159</v>
       </c>
@@ -25486,7 +25505,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="193"/>
+      <c r="A13" s="194"/>
       <c r="B13" s="128" t="s">
         <v>160</v>
       </c>
@@ -25495,7 +25514,7 @@
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="193"/>
+      <c r="A14" s="194"/>
       <c r="B14" s="139" t="s">
         <v>210</v>
       </c>
@@ -25507,7 +25526,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="193"/>
+      <c r="A15" s="194"/>
       <c r="B15" s="128" t="s">
         <v>177</v>
       </c>
@@ -25519,7 +25538,7 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="193"/>
+      <c r="A16" s="194"/>
       <c r="B16" s="128" t="s">
         <v>178</v>
       </c>
@@ -25528,7 +25547,7 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A17" s="194"/>
+      <c r="A17" s="195"/>
       <c r="B17" s="136" t="s">
         <v>161</v>
       </c>
@@ -25543,7 +25562,7 @@
       <c r="E18" s="94"/>
     </row>
     <row r="19" spans="1:5" collapsed="1">
-      <c r="A19" s="192" t="s">
+      <c r="A19" s="193" t="s">
         <v>209</v>
       </c>
       <c r="B19" s="131" t="s">
@@ -25552,7 +25571,7 @@
       <c r="C19" s="130"/>
     </row>
     <row r="20" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A20" s="193"/>
+      <c r="A20" s="194"/>
       <c r="B20" s="128" t="s">
         <v>159</v>
       </c>
@@ -25562,14 +25581,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A21" s="193"/>
+      <c r="A21" s="194"/>
       <c r="B21" s="128" t="s">
         <v>160</v>
       </c>
       <c r="C21" s="133"/>
     </row>
     <row r="22" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A22" s="193"/>
+      <c r="A22" s="194"/>
       <c r="B22" s="139" t="s">
         <v>210</v>
       </c>
@@ -25579,7 +25598,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A23" s="193"/>
+      <c r="A23" s="194"/>
       <c r="B23" s="128" t="s">
         <v>177</v>
       </c>
@@ -25589,14 +25608,14 @@
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1" outlineLevel="1">
-      <c r="A24" s="193"/>
+      <c r="A24" s="194"/>
       <c r="B24" s="128" t="s">
         <v>178</v>
       </c>
       <c r="C24" s="132"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A25" s="194"/>
+      <c r="A25" s="195"/>
       <c r="B25" s="136" t="s">
         <v>161</v>
       </c>
@@ -25609,7 +25628,7 @@
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A19:A25"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25640,17 +25659,17 @@
       <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="211" t="s">
+      <c r="A2" s="202" t="s">
         <v>189</v>
       </c>
-      <c r="B2" s="212"/>
+      <c r="B2" s="203"/>
       <c r="C2" s="120"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="213" t="s">
+      <c r="A3" s="204" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="212"/>
+      <c r="B3" s="203"/>
       <c r="C3" s="120"/>
     </row>
     <row r="4" spans="1:5">
@@ -25666,115 +25685,128 @@
       <c r="C5" s="120"/>
     </row>
     <row r="7" spans="1:5" ht="18.75">
-      <c r="A7" s="199" t="s">
+      <c r="A7" s="213" t="s">
         <v>192</v>
       </c>
-      <c r="B7" s="200"/>
+      <c r="B7" s="214"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="120"/>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="39" customHeight="1">
-      <c r="A9" s="201" t="s">
+      <c r="A9" s="211" t="s">
         <v>193</v>
       </c>
-      <c r="B9" s="202"/>
+      <c r="B9" s="212"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="203"/>
-      <c r="B10" s="204"/>
+      <c r="A10" s="198"/>
+      <c r="B10" s="199"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="200" t="s">
         <v>194</v>
       </c>
-      <c r="B11" s="196"/>
+      <c r="B11" s="201"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="195" t="s">
+      <c r="A12" s="200" t="s">
         <v>195</v>
       </c>
-      <c r="B12" s="196"/>
+      <c r="B12" s="201"/>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A13" s="195" t="s">
+      <c r="A13" s="200" t="s">
         <v>196</v>
       </c>
-      <c r="B13" s="196"/>
+      <c r="B13" s="201"/>
     </row>
     <row r="14" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="200" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="196"/>
+      <c r="B14" s="201"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1">
-      <c r="A15" s="195" t="s">
+      <c r="A15" s="200" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="196"/>
+      <c r="B15" s="201"/>
     </row>
     <row r="16" spans="1:5" ht="21" customHeight="1">
-      <c r="A16" s="195" t="s">
+      <c r="A16" s="200" t="s">
         <v>199</v>
       </c>
-      <c r="B16" s="196"/>
+      <c r="B16" s="201"/>
     </row>
     <row r="17" spans="1:2" ht="48.75" customHeight="1">
-      <c r="A17" s="197" t="s">
+      <c r="A17" s="196" t="s">
         <v>201</v>
       </c>
-      <c r="B17" s="198"/>
+      <c r="B17" s="197"/>
     </row>
     <row r="19" spans="1:2" ht="18.75">
-      <c r="A19" s="199" t="s">
+      <c r="A19" s="213" t="s">
         <v>203</v>
       </c>
-      <c r="B19" s="200"/>
+      <c r="B19" s="214"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="120"/>
       <c r="B20" s="9"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="201" t="s">
+      <c r="A21" s="211" t="s">
         <v>204</v>
       </c>
-      <c r="B21" s="202"/>
+      <c r="B21" s="212"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="203"/>
-      <c r="B22" s="204"/>
+      <c r="A22" s="198"/>
+      <c r="B22" s="199"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="195" t="s">
+      <c r="A23" s="200" t="s">
         <v>205</v>
       </c>
-      <c r="B23" s="196"/>
+      <c r="B23" s="201"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="195"/>
-      <c r="B24" s="196"/>
+      <c r="A24" s="200"/>
+      <c r="B24" s="201"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="195" t="s">
+      <c r="A25" s="200" t="s">
         <v>206</v>
       </c>
-      <c r="B25" s="196"/>
+      <c r="B25" s="201"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="195" t="s">
+      <c r="A26" s="200" t="s">
         <v>207</v>
       </c>
-      <c r="B26" s="196"/>
+      <c r="B26" s="201"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
+      <c r="A27" s="196"/>
+      <c r="B27" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
@@ -25785,19 +25817,6 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>

</xml_diff>

<commit_message>
Some more ram mapping, enemy stats
</commit_message>
<xml_diff>
--- a/DW3/DQ3.xlsx
+++ b/DW3/DQ3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="329">
   <si>
     <t>Notes</t>
   </si>
@@ -980,6 +980,72 @@
   </si>
   <si>
     <t>Enemy Current HP</t>
+  </si>
+  <si>
+    <t>Enemey 1 MP</t>
+  </si>
+  <si>
+    <t>Enemy 2 MP</t>
+  </si>
+  <si>
+    <t>Enemy 3 MP</t>
+  </si>
+  <si>
+    <t>Enemy 4 MP</t>
+  </si>
+  <si>
+    <t>Enemy 5 MP</t>
+  </si>
+  <si>
+    <t>Enemy 6 MP</t>
+  </si>
+  <si>
+    <t>Enemy 7 MP</t>
+  </si>
+  <si>
+    <t>Enemy 8 MP</t>
+  </si>
+  <si>
+    <t>Enemy 1 Agility</t>
+  </si>
+  <si>
+    <t>Enemy MP &amp; Agilty</t>
+  </si>
+  <si>
+    <t>Enemy 2 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 3 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 4 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 5 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 6 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 7 Agility</t>
+  </si>
+  <si>
+    <t>Enemy 8 Agility</t>
+  </si>
+  <si>
+    <t>Enemy Initialized and part of Member group</t>
+  </si>
+  <si>
+    <t>This 16 block is 2 byte values that relate to enemy initilized values and what group number they are in</t>
+  </si>
+  <si>
+    <t>Enemey Defense</t>
+  </si>
+  <si>
+    <t>Enemy 1 Defense</t>
+  </si>
+  <si>
+    <t>Enemy 2 Defense</t>
   </si>
 </sst>
 </file>
@@ -4769,8 +4835,8 @@
   <dimension ref="A1:H2186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1370" sqref="C1370"/>
+      <pane ySplit="2" topLeftCell="A1386" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1419" sqref="D1419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="3"/>
@@ -17370,461 +17436,645 @@
       </c>
       <c r="E1385" s="16"/>
     </row>
-    <row r="1386" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
+    <row r="1386" spans="1:5" ht="18" outlineLevel="1">
       <c r="A1386" s="76" t="s">
         <v>106</v>
       </c>
       <c r="B1386" s="90"/>
-      <c r="C1386" s="166"/>
+      <c r="C1386" s="166" t="s">
+        <v>316</v>
+      </c>
       <c r="D1386" s="167"/>
       <c r="E1386" s="167"/>
     </row>
-    <row r="1387" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1387" spans="1:5" outlineLevel="2">
       <c r="A1387" s="74">
         <v>0</v>
       </c>
-      <c r="B1387" s="88"/>
-      <c r="C1387" s="33"/>
-      <c r="D1387" s="15"/>
+      <c r="B1387" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1387" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1387" s="216" t="s">
+        <v>307</v>
+      </c>
       <c r="E1387" s="15"/>
     </row>
-    <row r="1388" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1388" spans="1:5" outlineLevel="2">
       <c r="A1388" s="74">
         <v>1</v>
       </c>
-      <c r="B1388" s="88"/>
-      <c r="C1388" s="33"/>
-      <c r="D1388" s="15"/>
+      <c r="B1388" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1388" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1388" s="216" t="s">
+        <v>308</v>
+      </c>
       <c r="E1388" s="15"/>
     </row>
-    <row r="1389" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1389" spans="1:5" outlineLevel="2">
       <c r="A1389" s="74">
         <v>2</v>
       </c>
-      <c r="B1389" s="88"/>
-      <c r="C1389" s="33"/>
-      <c r="D1389" s="15"/>
+      <c r="B1389" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1389" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1389" s="216" t="s">
+        <v>309</v>
+      </c>
       <c r="E1389" s="15"/>
     </row>
-    <row r="1390" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1390" spans="1:5" outlineLevel="2">
       <c r="A1390" s="74">
         <v>3</v>
       </c>
-      <c r="B1390" s="88"/>
-      <c r="C1390" s="33"/>
-      <c r="D1390" s="15"/>
+      <c r="B1390" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1390" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1390" s="216" t="s">
+        <v>310</v>
+      </c>
       <c r="E1390" s="15"/>
     </row>
-    <row r="1391" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1391" spans="1:5" outlineLevel="2">
       <c r="A1391" s="74">
         <v>4</v>
       </c>
-      <c r="B1391" s="88"/>
-      <c r="C1391" s="33"/>
-      <c r="D1391" s="15"/>
+      <c r="B1391" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1391" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1391" s="216" t="s">
+        <v>311</v>
+      </c>
       <c r="E1391" s="15"/>
     </row>
-    <row r="1392" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1392" spans="1:5" outlineLevel="2">
       <c r="A1392" s="74">
         <v>5</v>
       </c>
-      <c r="B1392" s="88"/>
-      <c r="C1392" s="33"/>
-      <c r="D1392" s="15"/>
+      <c r="B1392" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1392" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1392" s="216" t="s">
+        <v>312</v>
+      </c>
       <c r="E1392" s="15"/>
     </row>
-    <row r="1393" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1393" spans="1:5" outlineLevel="2">
       <c r="A1393" s="74">
         <v>6</v>
       </c>
-      <c r="B1393" s="88"/>
-      <c r="C1393" s="33"/>
-      <c r="D1393" s="15"/>
+      <c r="B1393" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1393" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1393" s="216" t="s">
+        <v>313</v>
+      </c>
       <c r="E1393" s="15"/>
     </row>
-    <row r="1394" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1394" spans="1:5" outlineLevel="2">
       <c r="A1394" s="74">
         <v>7</v>
       </c>
-      <c r="B1394" s="88"/>
-      <c r="C1394" s="33"/>
-      <c r="D1394" s="15"/>
+      <c r="B1394" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1394" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1394" s="216" t="s">
+        <v>314</v>
+      </c>
       <c r="E1394" s="15"/>
     </row>
-    <row r="1395" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1395" spans="1:5" outlineLevel="2">
       <c r="A1395" s="74">
         <v>8</v>
       </c>
-      <c r="B1395" s="88"/>
-      <c r="C1395" s="33"/>
-      <c r="D1395" s="15"/>
+      <c r="B1395" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1395" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1395" s="216" t="s">
+        <v>315</v>
+      </c>
       <c r="E1395" s="15"/>
     </row>
-    <row r="1396" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1396" spans="1:5" outlineLevel="2">
       <c r="A1396" s="74">
         <v>9</v>
       </c>
-      <c r="B1396" s="88"/>
-      <c r="C1396" s="33"/>
-      <c r="D1396" s="15"/>
+      <c r="B1396" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1396" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1396" s="216" t="s">
+        <v>317</v>
+      </c>
       <c r="E1396" s="15"/>
     </row>
-    <row r="1397" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1397" spans="1:5" outlineLevel="2">
       <c r="A1397" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1397" s="88"/>
-      <c r="C1397" s="33"/>
-      <c r="D1397" s="15"/>
+      <c r="B1397" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1397" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1397" s="216" t="s">
+        <v>318</v>
+      </c>
       <c r="E1397" s="15"/>
     </row>
-    <row r="1398" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1398" spans="1:5" outlineLevel="2">
       <c r="A1398" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B1398" s="88"/>
-      <c r="C1398" s="33"/>
-      <c r="D1398" s="15"/>
+      <c r="B1398" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1398" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1398" s="216" t="s">
+        <v>319</v>
+      </c>
       <c r="E1398" s="15"/>
     </row>
-    <row r="1399" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1399" spans="1:5" outlineLevel="2">
       <c r="A1399" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B1399" s="88"/>
-      <c r="C1399" s="33"/>
-      <c r="D1399" s="15"/>
+      <c r="B1399" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1399" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1399" s="216" t="s">
+        <v>320</v>
+      </c>
       <c r="E1399" s="15"/>
     </row>
-    <row r="1400" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1400" spans="1:5" outlineLevel="2">
       <c r="A1400" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B1400" s="88"/>
-      <c r="C1400" s="33"/>
-      <c r="D1400" s="15"/>
+      <c r="B1400" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1400" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1400" s="216" t="s">
+        <v>321</v>
+      </c>
       <c r="E1400" s="15"/>
     </row>
-    <row r="1401" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1401" spans="1:5" outlineLevel="2">
       <c r="A1401" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B1401" s="88"/>
-      <c r="C1401" s="33"/>
-      <c r="D1401" s="15"/>
+      <c r="B1401" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1401" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1401" s="216" t="s">
+        <v>322</v>
+      </c>
       <c r="E1401" s="15"/>
     </row>
-    <row r="1402" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1402" spans="1:5" outlineLevel="2">
       <c r="A1402" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B1402" s="88"/>
-      <c r="C1402" s="33"/>
-      <c r="D1402" s="15"/>
+      <c r="B1402" s="217" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1402" s="218" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1402" s="216" t="s">
+        <v>323</v>
+      </c>
       <c r="E1402" s="15"/>
     </row>
-    <row r="1403" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
+    <row r="1403" spans="1:5" ht="18" outlineLevel="1">
       <c r="A1403" s="73" t="s">
         <v>107</v>
       </c>
       <c r="B1403" s="87"/>
-      <c r="C1403" s="164"/>
+      <c r="C1403" s="164" t="s">
+        <v>326</v>
+      </c>
       <c r="D1403" s="165"/>
       <c r="E1403" s="165"/>
     </row>
-    <row r="1404" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1404" spans="1:5" outlineLevel="2">
       <c r="A1404" s="74">
         <v>0</v>
       </c>
-      <c r="B1404" s="88"/>
+      <c r="B1404" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1404" s="33"/>
-      <c r="D1404" s="15"/>
+      <c r="D1404" s="216" t="s">
+        <v>327</v>
+      </c>
       <c r="E1404" s="15"/>
     </row>
-    <row r="1405" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1405" spans="1:5" outlineLevel="2">
       <c r="A1405" s="74">
         <v>1</v>
       </c>
       <c r="B1405" s="88"/>
       <c r="C1405" s="33"/>
-      <c r="D1405" s="15"/>
+      <c r="D1405" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1405" s="15"/>
     </row>
-    <row r="1406" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1406" spans="1:5" outlineLevel="2">
       <c r="A1406" s="74">
         <v>2</v>
       </c>
-      <c r="B1406" s="88"/>
+      <c r="B1406" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1406" s="33"/>
-      <c r="D1406" s="15"/>
+      <c r="D1406" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1406" s="15"/>
     </row>
-    <row r="1407" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1407" spans="1:5" outlineLevel="2">
       <c r="A1407" s="74">
         <v>3</v>
       </c>
       <c r="B1407" s="88"/>
       <c r="C1407" s="33"/>
-      <c r="D1407" s="15"/>
+      <c r="D1407" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1407" s="15"/>
     </row>
-    <row r="1408" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1408" spans="1:5" outlineLevel="2">
       <c r="A1408" s="74">
         <v>4</v>
       </c>
-      <c r="B1408" s="88"/>
+      <c r="B1408" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1408" s="33"/>
-      <c r="D1408" s="15"/>
+      <c r="D1408" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1408" s="15"/>
     </row>
-    <row r="1409" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1409" spans="1:5" outlineLevel="2">
       <c r="A1409" s="74">
         <v>5</v>
       </c>
       <c r="B1409" s="88"/>
       <c r="C1409" s="33"/>
-      <c r="D1409" s="15"/>
+      <c r="D1409" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1409" s="15"/>
     </row>
-    <row r="1410" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1410" spans="1:5" outlineLevel="2">
       <c r="A1410" s="74">
         <v>6</v>
       </c>
-      <c r="B1410" s="88"/>
+      <c r="B1410" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1410" s="33"/>
-      <c r="D1410" s="15"/>
+      <c r="D1410" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1410" s="15"/>
     </row>
-    <row r="1411" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1411" spans="1:5" outlineLevel="2">
       <c r="A1411" s="74">
         <v>7</v>
       </c>
       <c r="B1411" s="88"/>
       <c r="C1411" s="33"/>
-      <c r="D1411" s="15"/>
+      <c r="D1411" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1411" s="15"/>
     </row>
-    <row r="1412" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1412" spans="1:5" outlineLevel="2">
       <c r="A1412" s="74">
         <v>8</v>
       </c>
-      <c r="B1412" s="88"/>
+      <c r="B1412" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1412" s="33"/>
-      <c r="D1412" s="15"/>
+      <c r="D1412" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1412" s="15"/>
     </row>
-    <row r="1413" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1413" spans="1:5" outlineLevel="2">
       <c r="A1413" s="74">
         <v>9</v>
       </c>
       <c r="B1413" s="88"/>
       <c r="C1413" s="33"/>
-      <c r="D1413" s="15"/>
+      <c r="D1413" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1413" s="15"/>
     </row>
-    <row r="1414" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1414" spans="1:5" outlineLevel="2">
       <c r="A1414" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1414" s="88"/>
+      <c r="B1414" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1414" s="33"/>
-      <c r="D1414" s="15"/>
+      <c r="D1414" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1414" s="15"/>
     </row>
-    <row r="1415" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1415" spans="1:5" outlineLevel="2">
       <c r="A1415" s="74" t="s">
         <v>3</v>
       </c>
       <c r="B1415" s="88"/>
       <c r="C1415" s="33"/>
-      <c r="D1415" s="15"/>
+      <c r="D1415" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1415" s="15"/>
     </row>
-    <row r="1416" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1416" spans="1:5" outlineLevel="2">
       <c r="A1416" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B1416" s="88"/>
+      <c r="B1416" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1416" s="33"/>
-      <c r="D1416" s="15"/>
+      <c r="D1416" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1416" s="15"/>
     </row>
-    <row r="1417" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1417" spans="1:5" outlineLevel="2">
       <c r="A1417" s="74" t="s">
         <v>5</v>
       </c>
       <c r="B1417" s="88"/>
       <c r="C1417" s="33"/>
-      <c r="D1417" s="15"/>
+      <c r="D1417" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1417" s="15"/>
     </row>
-    <row r="1418" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1418" spans="1:5" outlineLevel="2">
       <c r="A1418" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B1418" s="88"/>
+      <c r="B1418" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1418" s="33"/>
-      <c r="D1418" s="15"/>
+      <c r="D1418" s="216" t="s">
+        <v>328</v>
+      </c>
       <c r="E1418" s="15"/>
     </row>
-    <row r="1419" spans="1:5" ht="13.5" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="1419" spans="1:5" ht="13.5" outlineLevel="2" thickBot="1">
       <c r="A1419" s="75" t="s">
         <v>7</v>
       </c>
       <c r="B1419" s="89"/>
       <c r="C1419" s="34"/>
-      <c r="D1419" s="16"/>
+      <c r="D1419" s="216" t="s">
+        <v>237</v>
+      </c>
       <c r="E1419" s="16"/>
     </row>
-    <row r="1420" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
+    <row r="1420" spans="1:5" ht="18" outlineLevel="1">
       <c r="A1420" s="73" t="s">
         <v>108</v>
       </c>
       <c r="B1420" s="87"/>
-      <c r="C1420" s="164"/>
+      <c r="C1420" s="164" t="s">
+        <v>324</v>
+      </c>
       <c r="D1420" s="165"/>
       <c r="E1420" s="165"/>
     </row>
-    <row r="1421" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1421" spans="1:5" outlineLevel="2">
       <c r="A1421" s="74">
         <v>0</v>
       </c>
-      <c r="B1421" s="88"/>
+      <c r="B1421" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1421" s="33"/>
-      <c r="D1421" s="15"/>
+      <c r="D1421" s="216" t="s">
+        <v>325</v>
+      </c>
       <c r="E1421" s="15"/>
     </row>
-    <row r="1422" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1422" spans="1:5" outlineLevel="2">
       <c r="A1422" s="74">
         <v>1</v>
       </c>
-      <c r="B1422" s="88"/>
+      <c r="B1422" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1422" s="33"/>
       <c r="D1422" s="15"/>
       <c r="E1422" s="15"/>
     </row>
-    <row r="1423" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1423" spans="1:5" outlineLevel="2">
       <c r="A1423" s="74">
         <v>2</v>
       </c>
-      <c r="B1423" s="88"/>
+      <c r="B1423" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1423" s="33"/>
       <c r="D1423" s="15"/>
       <c r="E1423" s="15"/>
     </row>
-    <row r="1424" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1424" spans="1:5" outlineLevel="2">
       <c r="A1424" s="74">
         <v>3</v>
       </c>
-      <c r="B1424" s="88"/>
+      <c r="B1424" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1424" s="33"/>
       <c r="D1424" s="15"/>
       <c r="E1424" s="15"/>
     </row>
-    <row r="1425" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1425" spans="1:5" outlineLevel="2">
       <c r="A1425" s="74">
         <v>4</v>
       </c>
-      <c r="B1425" s="88"/>
+      <c r="B1425" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1425" s="33"/>
       <c r="D1425" s="15"/>
       <c r="E1425" s="15"/>
     </row>
-    <row r="1426" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1426" spans="1:5" outlineLevel="2">
       <c r="A1426" s="74">
         <v>5</v>
       </c>
-      <c r="B1426" s="88"/>
+      <c r="B1426" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1426" s="33"/>
       <c r="D1426" s="15"/>
       <c r="E1426" s="15"/>
     </row>
-    <row r="1427" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1427" spans="1:5" outlineLevel="2">
       <c r="A1427" s="74">
         <v>6</v>
       </c>
-      <c r="B1427" s="88"/>
+      <c r="B1427" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1427" s="33"/>
       <c r="D1427" s="15"/>
       <c r="E1427" s="15"/>
     </row>
-    <row r="1428" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1428" spans="1:5" outlineLevel="2">
       <c r="A1428" s="74">
         <v>7</v>
       </c>
-      <c r="B1428" s="88"/>
+      <c r="B1428" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1428" s="33"/>
       <c r="D1428" s="15"/>
       <c r="E1428" s="15"/>
     </row>
-    <row r="1429" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1429" spans="1:5" outlineLevel="2">
       <c r="A1429" s="74">
         <v>8</v>
       </c>
-      <c r="B1429" s="88"/>
+      <c r="B1429" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1429" s="33"/>
       <c r="D1429" s="15"/>
       <c r="E1429" s="15"/>
     </row>
-    <row r="1430" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1430" spans="1:5" outlineLevel="2">
       <c r="A1430" s="74">
         <v>9</v>
       </c>
-      <c r="B1430" s="88"/>
+      <c r="B1430" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1430" s="33"/>
       <c r="D1430" s="15"/>
       <c r="E1430" s="15"/>
     </row>
-    <row r="1431" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1431" spans="1:5" outlineLevel="2">
       <c r="A1431" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1431" s="88"/>
+      <c r="B1431" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1431" s="33"/>
       <c r="D1431" s="15"/>
       <c r="E1431" s="15"/>
     </row>
-    <row r="1432" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1432" spans="1:5" outlineLevel="2">
       <c r="A1432" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B1432" s="88"/>
+      <c r="B1432" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1432" s="33"/>
       <c r="D1432" s="15"/>
       <c r="E1432" s="15"/>
     </row>
-    <row r="1433" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1433" spans="1:5" outlineLevel="2">
       <c r="A1433" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B1433" s="88"/>
+      <c r="B1433" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1433" s="33"/>
       <c r="D1433" s="15"/>
       <c r="E1433" s="15"/>
     </row>
-    <row r="1434" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1434" spans="1:5" outlineLevel="2">
       <c r="A1434" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B1434" s="88"/>
+      <c r="B1434" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1434" s="33"/>
       <c r="D1434" s="15"/>
       <c r="E1434" s="15"/>
     </row>
-    <row r="1435" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1435" spans="1:5" outlineLevel="2">
       <c r="A1435" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B1435" s="88"/>
+      <c r="B1435" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1435" s="33"/>
       <c r="D1435" s="15"/>
       <c r="E1435" s="15"/>
     </row>
-    <row r="1436" spans="1:5" ht="13.5" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="1436" spans="1:5" ht="13.5" outlineLevel="2" thickBot="1">
       <c r="A1436" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="B1436" s="89"/>
+      <c r="B1436" s="217" t="s">
+        <v>296</v>
+      </c>
       <c r="C1436" s="34"/>
       <c r="D1436" s="16"/>
       <c r="E1436" s="16"/>

</xml_diff>

<commit_message>
DQ3 - some more memory mapping
</commit_message>
<xml_diff>
--- a/DW3/DQ3.xlsx
+++ b/DW3/DQ3.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="414">
   <si>
     <t>Notes</t>
   </si>
@@ -1030,9 +1030,6 @@
     <t>This 16 block is 2 byte values that relate to enemy initilized values and what group number they are in</t>
   </si>
   <si>
-    <t>Enemey Defense</t>
-  </si>
-  <si>
     <t>Enemy 1 Defense</t>
   </si>
   <si>
@@ -1280,6 +1277,30 @@
   </si>
   <si>
     <t>Party Info See http://www.gamefaqs.com/nes/587249-dragon-warrior-iii/faqs/2999 for details on meaning of values</t>
+  </si>
+  <si>
+    <t>Enemy Defense</t>
+  </si>
+  <si>
+    <t>Party Member 1 Battle Round decision</t>
+  </si>
+  <si>
+    <t>Party Member 2 Battle Round decision</t>
+  </si>
+  <si>
+    <t>Party Member 3 Battle Round decision</t>
+  </si>
+  <si>
+    <t>Party Member 4 Battle Round decision</t>
+  </si>
+  <si>
+    <t>80 = Attack, 90 = Use Spell, 21 = Parry</t>
+  </si>
+  <si>
+    <t>Party Battle decision</t>
+  </si>
+  <si>
+    <t>Sprite Memory (DMA)</t>
   </si>
 </sst>
 </file>
@@ -1724,7 +1745,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -2223,6 +2244,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2233,7 +2265,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2640,6 +2672,9 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="33" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -5069,8 +5104,8 @@
   <dimension ref="A1:H2186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1556" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2102" sqref="C2102:E2102"/>
+      <pane ySplit="2" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C242" sqref="C242:E242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="3"/>
@@ -5742,7 +5777,7 @@
       <c r="D71" s="16"/>
       <c r="E71" s="16"/>
     </row>
-    <row r="72" spans="1:5" ht="18" outlineLevel="1">
+    <row r="72" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
       <c r="A72" s="46" t="s">
         <v>12</v>
       </c>
@@ -5751,7 +5786,7 @@
       <c r="D72" s="169"/>
       <c r="E72" s="169"/>
     </row>
-    <row r="73" spans="1:5" outlineLevel="2">
+    <row r="73" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A73" s="47">
         <v>0</v>
       </c>
@@ -5760,7 +5795,7 @@
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
     </row>
-    <row r="74" spans="1:5" outlineLevel="2">
+    <row r="74" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A74" s="47">
         <v>1</v>
       </c>
@@ -5769,7 +5804,7 @@
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
     </row>
-    <row r="75" spans="1:5" outlineLevel="2">
+    <row r="75" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A75" s="47">
         <v>2</v>
       </c>
@@ -5778,7 +5813,7 @@
       <c r="D75" s="15"/>
       <c r="E75" s="15"/>
     </row>
-    <row r="76" spans="1:5" outlineLevel="2">
+    <row r="76" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A76" s="47">
         <v>3</v>
       </c>
@@ -5787,7 +5822,7 @@
       <c r="D76" s="15"/>
       <c r="E76" s="15"/>
     </row>
-    <row r="77" spans="1:5" outlineLevel="2">
+    <row r="77" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A77" s="47">
         <v>4</v>
       </c>
@@ -5796,7 +5831,7 @@
       <c r="D77" s="15"/>
       <c r="E77" s="15"/>
     </row>
-    <row r="78" spans="1:5" outlineLevel="2">
+    <row r="78" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A78" s="47">
         <v>5</v>
       </c>
@@ -5805,7 +5840,7 @@
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
     </row>
-    <row r="79" spans="1:5" outlineLevel="2">
+    <row r="79" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A79" s="47">
         <v>6</v>
       </c>
@@ -5814,7 +5849,7 @@
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
     </row>
-    <row r="80" spans="1:5" outlineLevel="2">
+    <row r="80" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A80" s="47">
         <v>7</v>
       </c>
@@ -5823,7 +5858,7 @@
       <c r="D80" s="15"/>
       <c r="E80" s="15"/>
     </row>
-    <row r="81" spans="1:5" outlineLevel="2">
+    <row r="81" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A81" s="47">
         <v>8</v>
       </c>
@@ -5832,7 +5867,7 @@
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
     </row>
-    <row r="82" spans="1:5" outlineLevel="2">
+    <row r="82" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A82" s="47">
         <v>9</v>
       </c>
@@ -5841,7 +5876,7 @@
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
     </row>
-    <row r="83" spans="1:5" outlineLevel="2">
+    <row r="83" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A83" s="47" t="s">
         <v>2</v>
       </c>
@@ -5850,7 +5885,7 @@
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
     </row>
-    <row r="84" spans="1:5" outlineLevel="2">
+    <row r="84" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A84" s="47" t="s">
         <v>3</v>
       </c>
@@ -5859,7 +5894,7 @@
       <c r="D84" s="15"/>
       <c r="E84" s="15"/>
     </row>
-    <row r="85" spans="1:5" outlineLevel="2">
+    <row r="85" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A85" s="47" t="s">
         <v>4</v>
       </c>
@@ -5868,7 +5903,7 @@
       <c r="D85" s="15"/>
       <c r="E85" s="15"/>
     </row>
-    <row r="86" spans="1:5" outlineLevel="2">
+    <row r="86" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A86" s="47" t="s">
         <v>5</v>
       </c>
@@ -5877,7 +5912,7 @@
       <c r="D86" s="15"/>
       <c r="E86" s="15"/>
     </row>
-    <row r="87" spans="1:5" outlineLevel="2">
+    <row r="87" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A87" s="47" t="s">
         <v>6</v>
       </c>
@@ -5886,7 +5921,7 @@
       <c r="D87" s="15"/>
       <c r="E87" s="15"/>
     </row>
-    <row r="88" spans="1:5" ht="13.5" outlineLevel="2" thickBot="1">
+    <row r="88" spans="1:5" ht="13.5" hidden="1" outlineLevel="2" thickBot="1">
       <c r="A88" s="48" t="s">
         <v>7</v>
       </c>
@@ -10044,7 +10079,9 @@
         <v>50</v>
       </c>
       <c r="B549" s="38"/>
-      <c r="C549" s="174"/>
+      <c r="C549" s="174" t="s">
+        <v>413</v>
+      </c>
       <c r="D549" s="175"/>
       <c r="E549" s="175"/>
     </row>
@@ -10053,9 +10090,11 @@
         <v>51</v>
       </c>
       <c r="B550" s="87"/>
-      <c r="C550" s="168"/>
-      <c r="D550" s="169"/>
-      <c r="E550" s="169"/>
+      <c r="C550" s="220" t="s">
+        <v>413</v>
+      </c>
+      <c r="D550" s="221"/>
+      <c r="E550" s="222"/>
     </row>
     <row r="551" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A551" s="59">
@@ -10206,7 +10245,9 @@
         <v>52</v>
       </c>
       <c r="B567" s="90"/>
-      <c r="C567" s="170"/>
+      <c r="C567" s="170" t="s">
+        <v>413</v>
+      </c>
       <c r="D567" s="171"/>
       <c r="E567" s="171"/>
     </row>
@@ -10359,9 +10400,11 @@
         <v>53</v>
       </c>
       <c r="B584" s="87"/>
-      <c r="C584" s="168"/>
-      <c r="D584" s="169"/>
-      <c r="E584" s="169"/>
+      <c r="C584" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D584" s="171"/>
+      <c r="E584" s="171"/>
     </row>
     <row r="585" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A585" s="59">
@@ -10512,9 +10555,11 @@
         <v>54</v>
       </c>
       <c r="B601" s="87"/>
-      <c r="C601" s="168"/>
-      <c r="D601" s="169"/>
-      <c r="E601" s="169"/>
+      <c r="C601" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D601" s="171"/>
+      <c r="E601" s="171"/>
     </row>
     <row r="602" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A602" s="59">
@@ -10665,9 +10710,11 @@
         <v>55</v>
       </c>
       <c r="B618" s="87"/>
-      <c r="C618" s="168"/>
-      <c r="D618" s="169"/>
-      <c r="E618" s="169"/>
+      <c r="C618" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D618" s="171"/>
+      <c r="E618" s="171"/>
     </row>
     <row r="619" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A619" s="59">
@@ -10818,9 +10865,11 @@
         <v>56</v>
       </c>
       <c r="B635" s="87"/>
-      <c r="C635" s="168"/>
-      <c r="D635" s="169"/>
-      <c r="E635" s="169"/>
+      <c r="C635" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D635" s="171"/>
+      <c r="E635" s="171"/>
     </row>
     <row r="636" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A636" s="59">
@@ -10971,9 +11020,11 @@
         <v>57</v>
       </c>
       <c r="B652" s="87"/>
-      <c r="C652" s="168"/>
-      <c r="D652" s="169"/>
-      <c r="E652" s="169"/>
+      <c r="C652" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D652" s="171"/>
+      <c r="E652" s="171"/>
     </row>
     <row r="653" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A653" s="59">
@@ -11124,9 +11175,11 @@
         <v>58</v>
       </c>
       <c r="B669" s="87"/>
-      <c r="C669" s="168"/>
-      <c r="D669" s="169"/>
-      <c r="E669" s="169"/>
+      <c r="C669" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D669" s="171"/>
+      <c r="E669" s="171"/>
     </row>
     <row r="670" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A670" s="59">
@@ -11277,9 +11330,11 @@
         <v>59</v>
       </c>
       <c r="B686" s="87"/>
-      <c r="C686" s="168"/>
-      <c r="D686" s="169"/>
-      <c r="E686" s="169"/>
+      <c r="C686" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D686" s="171"/>
+      <c r="E686" s="171"/>
     </row>
     <row r="687" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A687" s="59">
@@ -11430,9 +11485,11 @@
         <v>60</v>
       </c>
       <c r="B703" s="87"/>
-      <c r="C703" s="168"/>
-      <c r="D703" s="169"/>
-      <c r="E703" s="169"/>
+      <c r="C703" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D703" s="171"/>
+      <c r="E703" s="171"/>
     </row>
     <row r="704" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A704" s="59">
@@ -11583,9 +11640,11 @@
         <v>61</v>
       </c>
       <c r="B720" s="87"/>
-      <c r="C720" s="168"/>
-      <c r="D720" s="169"/>
-      <c r="E720" s="169"/>
+      <c r="C720" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D720" s="171"/>
+      <c r="E720" s="171"/>
     </row>
     <row r="721" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A721" s="59">
@@ -11736,9 +11795,11 @@
         <v>62</v>
       </c>
       <c r="B737" s="87"/>
-      <c r="C737" s="168"/>
-      <c r="D737" s="169"/>
-      <c r="E737" s="169"/>
+      <c r="C737" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D737" s="171"/>
+      <c r="E737" s="171"/>
     </row>
     <row r="738" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A738" s="59">
@@ -11889,9 +11950,11 @@
         <v>63</v>
       </c>
       <c r="B754" s="87"/>
-      <c r="C754" s="168"/>
-      <c r="D754" s="169"/>
-      <c r="E754" s="169"/>
+      <c r="C754" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D754" s="171"/>
+      <c r="E754" s="171"/>
     </row>
     <row r="755" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A755" s="59">
@@ -12042,9 +12105,11 @@
         <v>64</v>
       </c>
       <c r="B771" s="87"/>
-      <c r="C771" s="168"/>
-      <c r="D771" s="169"/>
-      <c r="E771" s="169"/>
+      <c r="C771" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D771" s="171"/>
+      <c r="E771" s="171"/>
     </row>
     <row r="772" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A772" s="59">
@@ -12195,9 +12260,11 @@
         <v>65</v>
       </c>
       <c r="B788" s="87"/>
-      <c r="C788" s="168"/>
-      <c r="D788" s="169"/>
-      <c r="E788" s="169"/>
+      <c r="C788" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D788" s="171"/>
+      <c r="E788" s="171"/>
     </row>
     <row r="789" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A789" s="59">
@@ -12348,9 +12415,11 @@
         <v>66</v>
       </c>
       <c r="B805" s="87"/>
-      <c r="C805" s="168"/>
-      <c r="D805" s="169"/>
-      <c r="E805" s="169"/>
+      <c r="C805" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="D805" s="171"/>
+      <c r="E805" s="171"/>
     </row>
     <row r="806" spans="1:5" hidden="1" outlineLevel="2">
       <c r="A806" s="59">
@@ -17927,7 +17996,7 @@
       </c>
       <c r="B1403" s="87"/>
       <c r="C1403" s="168" t="s">
-        <v>323</v>
+        <v>406</v>
       </c>
       <c r="D1403" s="169"/>
       <c r="E1403" s="169"/>
@@ -17941,7 +18010,7 @@
       </c>
       <c r="C1404" s="33"/>
       <c r="D1404" s="152" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E1404" s="15"/>
     </row>
@@ -17965,7 +18034,7 @@
       </c>
       <c r="C1406" s="33"/>
       <c r="D1406" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1406" s="15"/>
     </row>
@@ -17989,7 +18058,7 @@
       </c>
       <c r="C1408" s="33"/>
       <c r="D1408" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1408" s="15"/>
     </row>
@@ -18013,7 +18082,7 @@
       </c>
       <c r="C1410" s="33"/>
       <c r="D1410" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1410" s="15"/>
     </row>
@@ -18037,7 +18106,7 @@
       </c>
       <c r="C1412" s="33"/>
       <c r="D1412" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1412" s="15"/>
     </row>
@@ -18061,7 +18130,7 @@
       </c>
       <c r="C1414" s="33"/>
       <c r="D1414" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1414" s="15"/>
     </row>
@@ -18085,7 +18154,7 @@
       </c>
       <c r="C1416" s="33"/>
       <c r="D1416" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1416" s="15"/>
     </row>
@@ -18109,7 +18178,7 @@
       </c>
       <c r="C1418" s="33"/>
       <c r="D1418" s="152" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E1418" s="15"/>
     </row>
@@ -18313,16 +18382,18 @@
       <c r="D1436" s="16"/>
       <c r="E1436" s="16"/>
     </row>
-    <row r="1437" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
+    <row r="1437" spans="1:5" ht="18" outlineLevel="1">
       <c r="A1437" s="73" t="s">
         <v>109</v>
       </c>
       <c r="B1437" s="87"/>
-      <c r="C1437" s="168"/>
+      <c r="C1437" s="168" t="s">
+        <v>412</v>
+      </c>
       <c r="D1437" s="169"/>
       <c r="E1437" s="169"/>
     </row>
-    <row r="1438" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1438" spans="1:5" outlineLevel="2">
       <c r="A1438" s="74">
         <v>0</v>
       </c>
@@ -18331,7 +18402,7 @@
       <c r="D1438" s="15"/>
       <c r="E1438" s="15"/>
     </row>
-    <row r="1439" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1439" spans="1:5" outlineLevel="2">
       <c r="A1439" s="74">
         <v>1</v>
       </c>
@@ -18340,7 +18411,7 @@
       <c r="D1439" s="15"/>
       <c r="E1439" s="15"/>
     </row>
-    <row r="1440" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1440" spans="1:5" outlineLevel="2">
       <c r="A1440" s="74">
         <v>2</v>
       </c>
@@ -18349,7 +18420,7 @@
       <c r="D1440" s="15"/>
       <c r="E1440" s="15"/>
     </row>
-    <row r="1441" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1441" spans="1:5" outlineLevel="2">
       <c r="A1441" s="74">
         <v>3</v>
       </c>
@@ -18358,7 +18429,7 @@
       <c r="D1441" s="15"/>
       <c r="E1441" s="15"/>
     </row>
-    <row r="1442" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1442" spans="1:5" outlineLevel="2">
       <c r="A1442" s="74">
         <v>4</v>
       </c>
@@ -18367,7 +18438,7 @@
       <c r="D1442" s="15"/>
       <c r="E1442" s="15"/>
     </row>
-    <row r="1443" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1443" spans="1:5" outlineLevel="2">
       <c r="A1443" s="74">
         <v>5</v>
       </c>
@@ -18376,7 +18447,7 @@
       <c r="D1443" s="15"/>
       <c r="E1443" s="15"/>
     </row>
-    <row r="1444" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1444" spans="1:5" outlineLevel="2">
       <c r="A1444" s="74">
         <v>6</v>
       </c>
@@ -18385,7 +18456,7 @@
       <c r="D1444" s="15"/>
       <c r="E1444" s="15"/>
     </row>
-    <row r="1445" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1445" spans="1:5" outlineLevel="2">
       <c r="A1445" s="74">
         <v>7</v>
       </c>
@@ -18394,7 +18465,7 @@
       <c r="D1445" s="15"/>
       <c r="E1445" s="15"/>
     </row>
-    <row r="1446" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1446" spans="1:5" outlineLevel="2">
       <c r="A1446" s="74">
         <v>8</v>
       </c>
@@ -18403,7 +18474,7 @@
       <c r="D1446" s="15"/>
       <c r="E1446" s="15"/>
     </row>
-    <row r="1447" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1447" spans="1:5" outlineLevel="2">
       <c r="A1447" s="74">
         <v>9</v>
       </c>
@@ -18412,7 +18483,7 @@
       <c r="D1447" s="15"/>
       <c r="E1447" s="15"/>
     </row>
-    <row r="1448" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1448" spans="1:5" outlineLevel="2">
       <c r="A1448" s="74" t="s">
         <v>2</v>
       </c>
@@ -18421,7 +18492,7 @@
       <c r="D1448" s="15"/>
       <c r="E1448" s="15"/>
     </row>
-    <row r="1449" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1449" spans="1:5" outlineLevel="2">
       <c r="A1449" s="74" t="s">
         <v>3</v>
       </c>
@@ -18430,40 +18501,50 @@
       <c r="D1449" s="15"/>
       <c r="E1449" s="15"/>
     </row>
-    <row r="1450" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1450" spans="1:5" outlineLevel="2">
       <c r="A1450" s="74" t="s">
         <v>4</v>
       </c>
       <c r="B1450" s="88"/>
       <c r="C1450" s="33"/>
-      <c r="D1450" s="15"/>
-      <c r="E1450" s="15"/>
-    </row>
-    <row r="1451" spans="1:5" hidden="1" outlineLevel="2">
+      <c r="D1450" s="152" t="s">
+        <v>407</v>
+      </c>
+      <c r="E1450" s="152" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:5" outlineLevel="2">
       <c r="A1451" s="74" t="s">
         <v>5</v>
       </c>
       <c r="B1451" s="88"/>
       <c r="C1451" s="33"/>
-      <c r="D1451" s="15"/>
+      <c r="D1451" s="152" t="s">
+        <v>408</v>
+      </c>
       <c r="E1451" s="15"/>
     </row>
-    <row r="1452" spans="1:5" hidden="1" outlineLevel="2">
+    <row r="1452" spans="1:5" outlineLevel="2">
       <c r="A1452" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B1452" s="88"/>
       <c r="C1452" s="33"/>
-      <c r="D1452" s="15"/>
+      <c r="D1452" s="152" t="s">
+        <v>409</v>
+      </c>
       <c r="E1452" s="15"/>
     </row>
-    <row r="1453" spans="1:5" ht="13.5" hidden="1" outlineLevel="2" thickBot="1">
+    <row r="1453" spans="1:5" ht="13.5" outlineLevel="2" thickBot="1">
       <c r="A1453" s="75" t="s">
         <v>7</v>
       </c>
       <c r="B1453" s="89"/>
       <c r="C1453" s="34"/>
-      <c r="D1453" s="16"/>
+      <c r="D1453" s="155" t="s">
+        <v>410</v>
+      </c>
       <c r="E1453" s="16"/>
     </row>
     <row r="1454" spans="1:5" ht="18" outlineLevel="1" collapsed="1">
@@ -22612,7 +22693,7 @@
       </c>
       <c r="B1914" s="43"/>
       <c r="C1914" s="184" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D1914" s="185"/>
       <c r="E1914" s="185"/>
@@ -22623,7 +22704,7 @@
       </c>
       <c r="B1915" s="87"/>
       <c r="C1915" s="168" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D1915" s="169"/>
       <c r="E1915" s="169"/>
@@ -22636,10 +22717,10 @@
         <v>254</v>
       </c>
       <c r="C1916" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1916" s="152" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E1916" s="15"/>
     </row>
@@ -22651,10 +22732,10 @@
         <v>254</v>
       </c>
       <c r="C1917" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1917" s="152" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E1917" s="15"/>
     </row>
@@ -22666,10 +22747,10 @@
         <v>254</v>
       </c>
       <c r="C1918" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1918" s="152" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E1918" s="15"/>
     </row>
@@ -22681,10 +22762,10 @@
         <v>254</v>
       </c>
       <c r="C1919" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1919" s="152" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E1919" s="15"/>
     </row>
@@ -22696,10 +22777,10 @@
         <v>254</v>
       </c>
       <c r="C1920" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1920" s="152" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1920" s="15"/>
     </row>
@@ -22711,10 +22792,10 @@
         <v>254</v>
       </c>
       <c r="C1921" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1921" s="152" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E1921" s="15"/>
     </row>
@@ -22726,10 +22807,10 @@
         <v>254</v>
       </c>
       <c r="C1922" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1922" s="152" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E1922" s="15"/>
     </row>
@@ -22741,10 +22822,10 @@
         <v>254</v>
       </c>
       <c r="C1923" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1923" s="152" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E1923" s="15"/>
     </row>
@@ -22756,10 +22837,10 @@
         <v>254</v>
       </c>
       <c r="C1924" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1924" s="152" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E1924" s="15"/>
     </row>
@@ -22771,10 +22852,10 @@
         <v>254</v>
       </c>
       <c r="C1925" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1925" s="152" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E1925" s="15"/>
     </row>
@@ -22786,10 +22867,10 @@
         <v>254</v>
       </c>
       <c r="C1926" s="154" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1926" s="152" t="s">
         <v>327</v>
-      </c>
-      <c r="D1926" s="152" t="s">
-        <v>328</v>
       </c>
       <c r="E1926" s="15"/>
     </row>
@@ -22801,10 +22882,10 @@
         <v>254</v>
       </c>
       <c r="C1927" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1927" s="152" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E1927" s="15"/>
     </row>
@@ -22816,10 +22897,10 @@
         <v>254</v>
       </c>
       <c r="C1928" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1928" s="152" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E1928" s="15"/>
     </row>
@@ -22831,10 +22912,10 @@
         <v>254</v>
       </c>
       <c r="C1929" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1929" s="152" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E1929" s="15"/>
     </row>
@@ -22846,10 +22927,10 @@
         <v>254</v>
       </c>
       <c r="C1930" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1930" s="152" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E1930" s="15"/>
     </row>
@@ -22861,10 +22942,10 @@
         <v>254</v>
       </c>
       <c r="C1931" s="154" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D1931" s="155" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E1931" s="16"/>
     </row>
@@ -22874,7 +22955,7 @@
       </c>
       <c r="B1932" s="90"/>
       <c r="C1932" s="170" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D1932" s="171"/>
       <c r="E1932" s="171"/>
@@ -22886,7 +22967,7 @@
       <c r="B1933" s="88"/>
       <c r="C1933" s="33"/>
       <c r="D1933" s="152" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E1933" s="15"/>
     </row>
@@ -22897,7 +22978,7 @@
       <c r="B1934" s="88"/>
       <c r="C1934" s="33"/>
       <c r="D1934" s="152" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E1934" s="15"/>
     </row>
@@ -22908,7 +22989,7 @@
       <c r="B1935" s="88"/>
       <c r="C1935" s="33"/>
       <c r="D1935" s="152" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E1935" s="15"/>
     </row>
@@ -22919,7 +23000,7 @@
       <c r="B1936" s="88"/>
       <c r="C1936" s="33"/>
       <c r="D1936" s="152" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E1936" s="15"/>
     </row>
@@ -22930,7 +23011,7 @@
       <c r="B1937" s="88"/>
       <c r="C1937" s="33"/>
       <c r="D1937" s="152" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E1937" s="15"/>
     </row>
@@ -22941,7 +23022,7 @@
       <c r="B1938" s="88"/>
       <c r="C1938" s="33"/>
       <c r="D1938" s="152" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E1938" s="15"/>
     </row>
@@ -22952,7 +23033,7 @@
       <c r="B1939" s="88"/>
       <c r="C1939" s="33"/>
       <c r="D1939" s="152" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E1939" s="15"/>
     </row>
@@ -22963,7 +23044,7 @@
       <c r="B1940" s="88"/>
       <c r="C1940" s="33"/>
       <c r="D1940" s="152" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E1940" s="15"/>
     </row>
@@ -22974,7 +23055,7 @@
       <c r="B1941" s="88"/>
       <c r="C1941" s="33"/>
       <c r="D1941" s="152" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E1941" s="15"/>
     </row>
@@ -22985,7 +23066,7 @@
       <c r="B1942" s="88"/>
       <c r="C1942" s="33"/>
       <c r="D1942" s="152" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E1942" s="15"/>
     </row>
@@ -22996,7 +23077,7 @@
       <c r="B1943" s="88"/>
       <c r="C1943" s="33"/>
       <c r="D1943" s="152" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E1943" s="15"/>
     </row>
@@ -23007,7 +23088,7 @@
       <c r="B1944" s="88"/>
       <c r="C1944" s="33"/>
       <c r="D1944" s="152" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E1944" s="15"/>
     </row>
@@ -23268,7 +23349,7 @@
       </c>
       <c r="B1966" s="87"/>
       <c r="C1966" s="168" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D1966" s="169"/>
       <c r="E1966" s="169"/>
@@ -23424,7 +23505,7 @@
       <c r="B1979" s="153"/>
       <c r="C1979" s="154"/>
       <c r="D1979" s="152" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E1979" s="15"/>
     </row>
@@ -23435,7 +23516,7 @@
       <c r="B1980" s="88"/>
       <c r="C1980" s="33"/>
       <c r="D1980" s="152" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E1980" s="15"/>
     </row>
@@ -23446,7 +23527,7 @@
       <c r="B1981" s="88"/>
       <c r="C1981" s="33"/>
       <c r="D1981" s="152" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E1981" s="15"/>
     </row>
@@ -23457,7 +23538,7 @@
       <c r="B1982" s="89"/>
       <c r="C1982" s="34"/>
       <c r="D1982" s="155" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E1982" s="16"/>
     </row>
@@ -23467,7 +23548,7 @@
       </c>
       <c r="B1983" s="87"/>
       <c r="C1983" s="168" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D1983" s="169"/>
       <c r="E1983" s="169"/>
@@ -23479,7 +23560,7 @@
       <c r="B1984" s="88"/>
       <c r="C1984" s="33"/>
       <c r="D1984" s="152" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E1984" s="15"/>
     </row>
@@ -23490,7 +23571,7 @@
       <c r="B1985" s="88"/>
       <c r="C1985" s="33"/>
       <c r="D1985" s="152" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E1985" s="15"/>
     </row>
@@ -23501,7 +23582,7 @@
       <c r="B1986" s="88"/>
       <c r="C1986" s="33"/>
       <c r="D1986" s="152" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E1986" s="15"/>
     </row>
@@ -23512,7 +23593,7 @@
       <c r="B1987" s="88"/>
       <c r="C1987" s="33"/>
       <c r="D1987" s="152" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E1987" s="15"/>
     </row>
@@ -23527,7 +23608,7 @@
         <v>294</v>
       </c>
       <c r="D1988" s="152" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E1988" s="15"/>
     </row>
@@ -23564,7 +23645,7 @@
         <v>294</v>
       </c>
       <c r="D1991" s="152" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E1991" s="15"/>
     </row>
@@ -23601,7 +23682,7 @@
         <v>294</v>
       </c>
       <c r="D1994" s="152" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E1994" s="15"/>
     </row>
@@ -23638,7 +23719,7 @@
         <v>294</v>
       </c>
       <c r="D1997" s="152" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E1997" s="15"/>
     </row>
@@ -23670,7 +23751,7 @@
       </c>
       <c r="B2000" s="87"/>
       <c r="C2000" s="168" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D2000" s="169"/>
       <c r="E2000" s="169"/>
@@ -23684,7 +23765,7 @@
       </c>
       <c r="C2001" s="33"/>
       <c r="D2001" s="152" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E2001" s="15"/>
     </row>
@@ -23715,11 +23796,11 @@
         <v>3</v>
       </c>
       <c r="B2004" s="153" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2004" s="33"/>
       <c r="D2004" s="152" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E2004" s="15"/>
     </row>
@@ -23754,7 +23835,7 @@
       </c>
       <c r="C2007" s="33"/>
       <c r="D2007" s="152" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E2007" s="15"/>
     </row>
@@ -23789,7 +23870,7 @@
       </c>
       <c r="C2010" s="33"/>
       <c r="D2010" s="152" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E2010" s="15"/>
     </row>
@@ -23822,7 +23903,7 @@
       <c r="B2013" s="88"/>
       <c r="C2013" s="33"/>
       <c r="D2013" s="152" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E2013" s="15"/>
     </row>
@@ -23833,7 +23914,7 @@
       <c r="B2014" s="88"/>
       <c r="C2014" s="33"/>
       <c r="D2014" s="152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2014" s="15"/>
     </row>
@@ -23844,7 +23925,7 @@
       <c r="B2015" s="88"/>
       <c r="C2015" s="33"/>
       <c r="D2015" s="152" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2015" s="15"/>
     </row>
@@ -23855,7 +23936,7 @@
       <c r="B2016" s="89"/>
       <c r="C2016" s="34"/>
       <c r="D2016" s="155" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E2016" s="16"/>
     </row>
@@ -23865,7 +23946,7 @@
       </c>
       <c r="B2017" s="87"/>
       <c r="C2017" s="168" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D2017" s="169"/>
       <c r="E2017" s="169"/>
@@ -23877,7 +23958,7 @@
       <c r="B2018" s="88"/>
       <c r="C2018" s="33"/>
       <c r="D2018" s="152" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E2018" s="15"/>
     </row>
@@ -23888,7 +23969,7 @@
       <c r="B2019" s="88"/>
       <c r="C2019" s="33"/>
       <c r="D2019" s="152" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2019" s="15"/>
     </row>
@@ -23899,7 +23980,7 @@
       <c r="B2020" s="88"/>
       <c r="C2020" s="33"/>
       <c r="D2020" s="152" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2020" s="15"/>
     </row>
@@ -23910,7 +23991,7 @@
       <c r="B2021" s="88"/>
       <c r="C2021" s="33"/>
       <c r="D2021" s="152" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2021" s="15"/>
     </row>
@@ -23921,7 +24002,7 @@
       <c r="B2022" s="88"/>
       <c r="C2022" s="33"/>
       <c r="D2022" s="152" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E2022" s="15"/>
     </row>
@@ -23932,7 +24013,7 @@
       <c r="B2023" s="88"/>
       <c r="C2023" s="33"/>
       <c r="D2023" s="152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2023" s="15"/>
     </row>
@@ -23943,7 +24024,7 @@
       <c r="B2024" s="88"/>
       <c r="C2024" s="33"/>
       <c r="D2024" s="152" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2024" s="15"/>
     </row>
@@ -23954,7 +24035,7 @@
       <c r="B2025" s="88"/>
       <c r="C2025" s="33"/>
       <c r="D2025" s="152" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E2025" s="15"/>
     </row>
@@ -23965,7 +24046,7 @@
       <c r="B2026" s="88"/>
       <c r="C2026" s="33"/>
       <c r="D2026" s="152" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E2026" s="15"/>
     </row>
@@ -23976,7 +24057,7 @@
       <c r="B2027" s="88"/>
       <c r="C2027" s="33"/>
       <c r="D2027" s="152" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2027" s="15"/>
     </row>
@@ -23987,7 +24068,7 @@
       <c r="B2028" s="88"/>
       <c r="C2028" s="33"/>
       <c r="D2028" s="152" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2028" s="15"/>
     </row>
@@ -23998,7 +24079,7 @@
       <c r="B2029" s="88"/>
       <c r="C2029" s="33"/>
       <c r="D2029" s="152" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2029" s="15"/>
     </row>
@@ -24009,7 +24090,7 @@
       <c r="B2030" s="88"/>
       <c r="C2030" s="33"/>
       <c r="D2030" s="152" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E2030" s="15"/>
     </row>
@@ -24020,7 +24101,7 @@
       <c r="B2031" s="88"/>
       <c r="C2031" s="33"/>
       <c r="D2031" s="152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2031" s="15"/>
     </row>
@@ -24031,7 +24112,7 @@
       <c r="B2032" s="88"/>
       <c r="C2032" s="33"/>
       <c r="D2032" s="152" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2032" s="15"/>
     </row>
@@ -24042,7 +24123,7 @@
       <c r="B2033" s="89"/>
       <c r="C2033" s="34"/>
       <c r="D2033" s="152" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E2033" s="16"/>
     </row>
@@ -24052,7 +24133,7 @@
       </c>
       <c r="B2034" s="87"/>
       <c r="C2034" s="168" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D2034" s="169"/>
       <c r="E2034" s="169"/>
@@ -24064,7 +24145,7 @@
       <c r="B2035" s="88"/>
       <c r="C2035" s="33"/>
       <c r="D2035" s="152" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E2035" s="15"/>
     </row>
@@ -24075,7 +24156,7 @@
       <c r="B2036" s="88"/>
       <c r="C2036" s="33"/>
       <c r="D2036" s="152" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2036" s="15"/>
     </row>
@@ -24086,7 +24167,7 @@
       <c r="B2037" s="88"/>
       <c r="C2037" s="33"/>
       <c r="D2037" s="152" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2037" s="15"/>
     </row>
@@ -24097,7 +24178,7 @@
       <c r="B2038" s="88"/>
       <c r="C2038" s="33"/>
       <c r="D2038" s="152" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2038" s="15"/>
     </row>
@@ -24108,7 +24189,7 @@
       <c r="B2039" s="88"/>
       <c r="C2039" s="33"/>
       <c r="D2039" s="152" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E2039" s="15"/>
     </row>
@@ -24119,7 +24200,7 @@
       <c r="B2040" s="88"/>
       <c r="C2040" s="33"/>
       <c r="D2040" s="152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2040" s="15"/>
     </row>
@@ -24130,7 +24211,7 @@
       <c r="B2041" s="88"/>
       <c r="C2041" s="33"/>
       <c r="D2041" s="152" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E2041" s="15"/>
     </row>
@@ -24141,7 +24222,7 @@
       <c r="B2042" s="88"/>
       <c r="C2042" s="33"/>
       <c r="D2042" s="152" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E2042" s="15"/>
     </row>
@@ -24152,7 +24233,7 @@
       <c r="B2043" s="88"/>
       <c r="C2043" s="33"/>
       <c r="D2043" s="152" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E2043" s="15"/>
     </row>
@@ -24163,7 +24244,7 @@
       <c r="B2044" s="88"/>
       <c r="C2044" s="33"/>
       <c r="D2044" s="152" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E2044" s="15"/>
     </row>
@@ -24174,7 +24255,7 @@
       <c r="B2045" s="88"/>
       <c r="C2045" s="33"/>
       <c r="D2045" s="152" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E2045" s="15"/>
     </row>
@@ -24185,7 +24266,7 @@
       <c r="B2046" s="88"/>
       <c r="C2046" s="33"/>
       <c r="D2046" s="152" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E2046" s="15"/>
     </row>
@@ -24468,7 +24549,7 @@
       </c>
       <c r="B2068" s="87"/>
       <c r="C2068" s="168" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D2068" s="169"/>
       <c r="E2068" s="169"/>
@@ -24634,14 +24715,14 @@
         <v>4</v>
       </c>
       <c r="B2081" s="153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C2081" s="154"/>
       <c r="D2081" s="152" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2081" s="152" t="s">
         <v>383</v>
-      </c>
-      <c r="E2081" s="152" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="2082" spans="1:5" hidden="1" outlineLevel="2">
@@ -24673,7 +24754,7 @@
       <c r="B2084" s="89"/>
       <c r="C2084" s="34"/>
       <c r="D2084" s="155" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2084" s="16"/>
     </row>
@@ -24683,7 +24764,7 @@
       </c>
       <c r="B2085" s="87"/>
       <c r="C2085" s="168" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D2085" s="169"/>
       <c r="E2085" s="169"/>
@@ -24693,11 +24774,11 @@
         <v>0</v>
       </c>
       <c r="B2086" s="153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C2086" s="33"/>
       <c r="D2086" s="152" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E2086" s="15"/>
     </row>
@@ -24708,7 +24789,7 @@
       <c r="B2087" s="88"/>
       <c r="C2087" s="33"/>
       <c r="D2087" s="152" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2087" s="15"/>
     </row>
@@ -24719,7 +24800,7 @@
       <c r="B2088" s="88"/>
       <c r="C2088" s="33"/>
       <c r="D2088" s="152" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E2088" s="15"/>
     </row>
@@ -24730,7 +24811,7 @@
       <c r="B2089" s="88"/>
       <c r="C2089" s="33"/>
       <c r="D2089" s="152" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E2089" s="15"/>
     </row>
@@ -24741,7 +24822,7 @@
       <c r="B2090" s="88"/>
       <c r="C2090" s="33"/>
       <c r="D2090" s="152" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E2090" s="15"/>
     </row>
@@ -24774,7 +24855,7 @@
       <c r="B2093" s="88"/>
       <c r="C2093" s="33"/>
       <c r="D2093" s="152" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2093" s="15"/>
     </row>
@@ -24785,7 +24866,7 @@
       <c r="B2094" s="88"/>
       <c r="C2094" s="33"/>
       <c r="D2094" s="152" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E2094" s="15"/>
     </row>
@@ -24796,7 +24877,7 @@
       <c r="B2095" s="88"/>
       <c r="C2095" s="33"/>
       <c r="D2095" s="152" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2095" s="15"/>
     </row>
@@ -24807,7 +24888,7 @@
       <c r="B2096" s="88"/>
       <c r="C2096" s="33"/>
       <c r="D2096" s="152" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E2096" s="15"/>
     </row>
@@ -24818,7 +24899,7 @@
       <c r="B2097" s="88"/>
       <c r="C2097" s="33"/>
       <c r="D2097" s="152" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E2097" s="15"/>
     </row>
@@ -24829,7 +24910,7 @@
       <c r="B2098" s="88"/>
       <c r="C2098" s="33"/>
       <c r="D2098" s="152" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E2098" s="15"/>
     </row>
@@ -24862,7 +24943,7 @@
       <c r="B2101" s="89"/>
       <c r="C2101" s="34"/>
       <c r="D2101" s="155" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2101" s="16"/>
     </row>
@@ -24872,7 +24953,7 @@
       </c>
       <c r="B2102" s="87"/>
       <c r="C2102" s="168" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D2102" s="169"/>
       <c r="E2102" s="169"/>
@@ -24882,11 +24963,11 @@
         <v>0</v>
       </c>
       <c r="B2103" s="153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C2103" s="33"/>
       <c r="D2103" s="152" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E2103" s="15"/>
     </row>
@@ -24897,7 +24978,7 @@
       <c r="B2104" s="88"/>
       <c r="C2104" s="33"/>
       <c r="D2104" s="152" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2104" s="15"/>
     </row>
@@ -24908,7 +24989,7 @@
       <c r="B2105" s="88"/>
       <c r="C2105" s="33"/>
       <c r="D2105" s="152" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E2105" s="15"/>
     </row>
@@ -24919,7 +25000,7 @@
       <c r="B2106" s="88"/>
       <c r="C2106" s="33"/>
       <c r="D2106" s="152" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E2106" s="15"/>
     </row>
@@ -24928,11 +25009,11 @@
         <v>4</v>
       </c>
       <c r="B2107" s="153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C2107" s="33"/>
       <c r="D2107" s="152" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2107" s="15"/>
     </row>
@@ -24965,7 +25046,7 @@
       <c r="B2110" s="88"/>
       <c r="C2110" s="33"/>
       <c r="D2110" s="152" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2110" s="15"/>
     </row>
@@ -24976,7 +25057,7 @@
       <c r="B2111" s="88"/>
       <c r="C2111" s="33"/>
       <c r="D2111" s="152" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E2111" s="15"/>
     </row>
@@ -24987,7 +25068,7 @@
       <c r="B2112" s="88"/>
       <c r="C2112" s="33"/>
       <c r="D2112" s="152" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E2112" s="15"/>
     </row>
@@ -24998,7 +25079,7 @@
       <c r="B2113" s="88"/>
       <c r="C2113" s="33"/>
       <c r="D2113" s="152" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E2113" s="15"/>
     </row>
@@ -25009,7 +25090,7 @@
       <c r="B2114" s="88"/>
       <c r="C2114" s="33"/>
       <c r="D2114" s="152" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E2114" s="15"/>
     </row>
@@ -25055,7 +25136,7 @@
       <c r="B2118" s="89"/>
       <c r="C2118" s="34"/>
       <c r="D2118" s="155" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E2118" s="16"/>
     </row>

</xml_diff>